<commit_message>
on presentation 14.03.25 stable
</commit_message>
<xml_diff>
--- a/data_after_OHE.xlsx
+++ b/data_after_OHE.xlsx
@@ -483,7 +483,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>bfdbc6ea-8ced-4255-a32b-00f3a1b03102</t>
+          <t>ab2f1d60-8403-4e45-84d7-1c66a1bf4390</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -517,7 +517,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>3616e635-4513-4802-83d7-e1942a020e33</t>
+          <t>68020565-e341-4e9f-a7d4-c746d6811023</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -551,7 +551,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>2f624d5c-b2de-44f7-a3da-8346bd18ad47</t>
+          <t>bda0db16-9462-4575-8d6e-e63f48c486de</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -585,7 +585,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>cd73dc1c-b8da-413f-ab85-011c33351341</t>
+          <t>7e8e027a-ea15-4c49-8d50-9a110084c6b7</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -619,7 +619,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>871e061f-33d6-4ea6-a1b8-2910f0ef7937</t>
+          <t>8e13475e-ee49-4f8d-9adb-7123ad9fed27</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -653,7 +653,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>51623f46-224d-4896-855d-baa436318e9e</t>
+          <t>4f3e427c-ce2f-4048-bebe-0ab229e7c104</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -687,7 +687,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>1e7626a6-3725-4caf-b9b9-fdad902f82dc</t>
+          <t>da1e9057-174d-466b-acf5-a86e8e0bf27c</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -721,7 +721,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>e8170e32-3427-48f9-901e-6723a6ec8795</t>
+          <t>f0c89bbd-1d76-43bd-a647-7816f46d85e1</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -755,7 +755,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>532186e4-1049-4b1f-a203-26e5ab12f932</t>
+          <t>f892db18-7ca0-40cc-a43a-2254c1a2c829</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -789,7 +789,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>3d0f377f-dafc-4369-9dc0-469658ab4e0f</t>
+          <t>d4bd943b-2079-4b9d-abbe-88317a7220e0</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -823,7 +823,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>828f303e-f67d-43e4-871e-f53f7552a0a0</t>
+          <t>03390cb5-c1c8-4401-8d95-0dbdfe5ff08b</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -857,7 +857,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>0ff6f6c9-7e25-4d93-a083-f0be9077db57</t>
+          <t>41fb3a89-ea3b-457c-bd02-440d061a2a98</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -891,7 +891,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>181d21b8-e310-41aa-a2bf-9c3d6de8e43c</t>
+          <t>06e955b2-f3a7-4902-b04b-716527291dee</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -925,7 +925,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>51e14c98-c8c2-406c-b9b5-b6e4c6c050b9</t>
+          <t>e40c260b-2d63-4506-bb8a-8781857658d6</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -959,7 +959,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>88f7459f-46ec-4d6b-b46e-dade18207505</t>
+          <t>1b08eeab-26a4-4a07-91c0-8256ea080c35</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -993,7 +993,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>6f4a190e-ed11-474a-8bbe-d8c2d9bd184e</t>
+          <t>1f85a1f9-e2a4-4d12-b056-52406be4a55e</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1027,7 +1027,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>ec19b4d3-a6aa-4d64-b071-0e6d5171f31e</t>
+          <t>8e266dfe-c166-487f-851e-2d10484f1bd9</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1061,7 +1061,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>7faeefd2-d69c-4f3f-9329-b0aa423d193a</t>
+          <t>2ad48434-dddd-4c5d-8e4f-27e45a66ea15</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1095,7 +1095,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>c45b18f4-c8ec-4299-bf10-89fb629cd3fa</t>
+          <t>267d3814-ec92-4d3d-a95a-a1251a411573</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1129,7 +1129,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>cc82674e-6a5a-4aa2-8e39-c11a9015d406</t>
+          <t>9920261e-7983-4bf9-b90c-63cf6b8b7758</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1163,7 +1163,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>4775768a-381e-46bf-8bd4-aacdd549488f</t>
+          <t>4e3e0788-b96f-4611-a02c-443995995728</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1197,7 +1197,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>72f32812-1d3b-4c58-b6dc-0bf0b28c6ca7</t>
+          <t>4dd453bb-bc8e-42bf-b8ff-9a9e4b135d98</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1231,7 +1231,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>7c1c9973-1726-4ccd-883b-573774799716</t>
+          <t>d51c9216-4853-4181-99fe-0b915f505021</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1265,7 +1265,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>f407dfcb-1a28-4b91-b5a6-fd4106dfbbee</t>
+          <t>89b7106e-9e6a-43f0-8b82-75b4ea355b08</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1299,7 +1299,7 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>e383efa1-9db2-4cb9-85d4-151e27fedb55</t>
+          <t>94fb619d-7773-4bbc-bec9-9aa75b0ddf21</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1333,7 +1333,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>3963bc61-72a0-4ecc-b29f-228cc9f57197</t>
+          <t>793045ad-96e5-4d7f-ab27-275463a7f7ef</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1367,7 +1367,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>fba10773-1574-461e-93e7-b1c8db9239b7</t>
+          <t>8cba5378-6b4f-40f4-bd27-cc6de43a8c0c</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1401,7 +1401,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>2cf30a38-d0e8-4d4d-8b86-6ab1bc586984</t>
+          <t>27ecae6c-dac5-49ca-acee-6747c95e09ad</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1435,7 +1435,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>24805f33-04b8-4f84-adfb-9af0d57b5051</t>
+          <t>dbf6e9da-84b1-4aec-9ef5-ee14cd7ad86a</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1469,7 +1469,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>4ac4753c-bc14-4a91-b5cf-42a53246b5ad</t>
+          <t>44ee3023-b0e1-4d99-8a22-3f8f6847ad73</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1503,7 +1503,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>2ae0bc5c-2120-4f23-97d0-bb1ec1d391af</t>
+          <t>39a3f519-8e0a-443e-9610-1620c1c66d71</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1537,7 +1537,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>e2dd443b-0296-4154-b206-64b6f4f88d1c</t>
+          <t>4df4bd19-796b-476a-ad62-8bb3bc1e9200</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1571,7 +1571,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>e89a5970-6379-442e-83ca-6becc95b6947</t>
+          <t>5e149d05-b3fa-4696-a230-ab482be5dbe2</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1605,7 +1605,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>6162e84e-9cf4-44ff-9ac6-1ccbfcd4ac1e</t>
+          <t>2dc65ade-b30d-4071-b9b2-940aa78d8af8</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1639,7 +1639,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>53f4c5d5-039f-413d-8f6a-e2193227d75f</t>
+          <t>33c2f638-ee42-4192-b341-322a074780e9</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1673,7 +1673,7 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>9ce591fc-4072-45b7-b386-1afe1a4a6a4f</t>
+          <t>5cf0dece-a482-42bc-b1e6-edf75e4a9a67</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1707,7 +1707,7 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>bb7e15b9-ab70-4622-9c0f-e16b534f57b9</t>
+          <t>f7b19fda-3fec-4f46-b273-0dad13549966</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1741,7 +1741,7 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>a8f49b47-e45e-4ba7-b01b-cb0c7667ba6c</t>
+          <t>f6dbc3ec-3981-4e33-a6b9-5990df6ead1e</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1775,7 +1775,7 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>dd292d2c-bde2-41a3-b575-192ce2102d16</t>
+          <t>173ad083-ce2b-444b-a80b-a7228f5c598c</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1809,7 +1809,7 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>764382b8-9205-45e3-aced-da39f5da0021</t>
+          <t>4207709b-5567-4a1e-a01a-ab6ff7c55bf8</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1843,7 +1843,7 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>c3fbeae0-7db6-4248-8744-05a2180712fa</t>
+          <t>65e508a9-03dc-4194-8804-f99ecd1f9917</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1877,7 +1877,7 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>b26d3ba9-3df7-41fd-b9fd-ce4899ba8f5c</t>
+          <t>d126079c-dd3a-4a17-961b-93969d943eb5</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1911,7 +1911,7 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>ae9b25bf-4991-4c76-9b4a-c70fb7e2a9e3</t>
+          <t>f2e08bac-c3e4-4704-8559-c629df87faca</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1945,7 +1945,7 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>76cb4ee8-b0c9-42b2-9e3f-539a54799c92</t>
+          <t>bbacda83-5477-4548-9c0e-443bb71c94cf</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1979,7 +1979,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>f95ef731-6c20-4fcf-94fb-bb24a9fb834e</t>
+          <t>ea4a5311-2fbb-451c-8fd5-daea90bfa6b0</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -2013,7 +2013,7 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>9fdea7bc-408c-4eda-841c-8fa6c30ebd17</t>
+          <t>a5f29874-cf1c-4161-8d85-a2b0931d42e8</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -2047,7 +2047,7 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>9e2fcb15-5a11-4fe0-b37b-f972e2f472f7</t>
+          <t>c6c9a636-3c30-47fd-9df3-d54ee3855990</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -2081,7 +2081,7 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>fb33d5f2-0f80-4237-9c8c-3d4d4d90bf9c</t>
+          <t>c0a72276-123e-47c8-b6a0-64d1673d2e19</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -2115,7 +2115,7 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>5a25ac09-8a97-40a4-9b92-d62ef9b0a967</t>
+          <t>29ac76f1-8f31-4deb-a846-63c4725cc36c</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -2149,7 +2149,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>552c9659-18b1-4172-8036-b4fb76dc5873</t>
+          <t>dcf8dbb2-cd36-474c-ba52-c4cfa930ae44</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -2183,7 +2183,7 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>e948dd0d-eb3d-457d-949a-3d53ee3f393b</t>
+          <t>4d19b2d7-773a-48d5-ae98-1f4cd89a27bd</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -2217,7 +2217,7 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>381b5855-84f6-457e-b97b-aa8e005c5a62</t>
+          <t>e0432c3f-062c-4c22-9626-fb8a1670331e</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -2251,7 +2251,7 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>cc712f61-fc0a-43f5-8479-327801a7ada5</t>
+          <t>9c43e645-edbf-4c78-847f-4eee7338a9c7</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -2285,7 +2285,7 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>bae01c89-5fba-4a20-a4fe-7504c3417e7e</t>
+          <t>69ce5aee-fd9b-43a6-8f43-2393f3f3242b</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -2319,7 +2319,7 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>9760e8f1-73cc-4c14-9c23-dd422bf21bba</t>
+          <t>73fa90c0-3a3d-4b6a-bbe6-8bd1a9dd2043</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -2353,7 +2353,7 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>de6517f5-b62f-4bcc-99cc-d2439fb28705</t>
+          <t>9767a9a1-ba51-4c17-81a0-365d46ef3768</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -2387,7 +2387,7 @@
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>a18a3034-967d-4d51-aaae-7d87ea6ef0d5</t>
+          <t>7b4b8534-1143-40d0-ba08-1c43ea72a8e3</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -2421,7 +2421,7 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>78860dc2-b8c4-4bc9-979b-17b89b465615</t>
+          <t>f48904f7-7909-43df-b591-6043fb6cf65c</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -2455,7 +2455,7 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>4040c599-b72d-469a-81c3-360e0f4bc9fd</t>
+          <t>d1a90533-f7ea-46dd-af36-f5704b042e04</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -2489,7 +2489,7 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>2ea8df0a-dfec-4cf8-9c5c-b005e30d5a91</t>
+          <t>7d89d0e4-f529-4cc8-8703-131173ef368e</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -2523,7 +2523,7 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>22b792e3-5210-47cf-b20a-d491556f2a35</t>
+          <t>a731e937-d3b4-4cb2-a311-b88025caf0e6</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -2557,7 +2557,7 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>2125a5d4-8261-4d6e-b713-9b7eeb40bbae</t>
+          <t>bcb6fd53-44b8-4b05-8c7a-f6a7716b2c29</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -2591,7 +2591,7 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>0d0ced3b-9c66-450f-a838-624cd9d8bbd2</t>
+          <t>a010abe7-6c1c-4b06-b9df-77cc8715b50f</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -2625,7 +2625,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>094649d9-f257-4fb0-8ddd-e58ecd2a69be</t>
+          <t>c5fb4491-dd50-4cc6-b3f3-b22b73bed3dc</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -2659,7 +2659,7 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>4d22b04a-1ed1-4607-9a26-c90ab37593e1</t>
+          <t>05209005-b769-4e5b-a78f-0d84874cb374</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -2693,7 +2693,7 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>65093781-41a1-4ade-8277-615c60661dbb</t>
+          <t>83a910cf-d482-4ce3-a602-000fde169776</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -2727,7 +2727,7 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>800da61e-31ee-485f-b302-b76595968570</t>
+          <t>b6388ae5-c8e0-4e71-aa9c-897b1963a662</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -2761,7 +2761,7 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>566dcb40-5e94-494f-8955-021e04dec689</t>
+          <t>5c2b2176-4662-4d96-8db6-de012ec8fd5c</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -2795,7 +2795,7 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>2f954ebc-97e9-46d0-b0e6-f2f1945b4e3b</t>
+          <t>88b18576-1ab4-4c3f-860f-9e222718474b</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -2829,7 +2829,7 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>cb35beb8-efe3-4054-8d63-87713359db05</t>
+          <t>53a4590f-a80d-4bdb-b7a2-d5ad74af9407</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -2863,7 +2863,7 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>c93d3511-e6c6-4139-876d-c32fcb24a5d1</t>
+          <t>074c6de4-36b2-449a-901c-a945b406b56a</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -2897,7 +2897,7 @@
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>347e5840-35b9-4292-87bd-475a4c224402</t>
+          <t>cc79f4a9-4558-4772-88d5-ac892248ddb0</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -2931,7 +2931,7 @@
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>9e86b939-e8a9-484a-b2b6-202ac1ea41df</t>
+          <t>02e2e5f6-45f4-428f-abbb-4c0e0b0b9598</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -2965,7 +2965,7 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>f21a555a-fdf0-47b8-a80c-d0a4ff2086bb</t>
+          <t>7a296875-cddd-448d-b8dc-74361d1f100d</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -2999,7 +2999,7 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>110ea71b-2443-495c-8270-f74353bf07d3</t>
+          <t>3686694e-4c41-407d-8c20-48278108a1a6</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -3033,7 +3033,7 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>c435f2fc-ca8c-4633-9e51-f9d44d71144c</t>
+          <t>3b2e64c9-3bc3-4d4e-8972-d40e245bf8fc</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -3067,7 +3067,7 @@
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>eb163ecd-393f-45e6-b8d6-0298d7a4fee5</t>
+          <t>388e7ea8-2514-40f7-b46b-a5abfc3eafa1</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -3101,7 +3101,7 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>c2b0d9ad-b087-43b4-be4f-ba0a3d9fa312</t>
+          <t>db7b9251-4894-4e45-b6d2-b167457a35c6</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -3135,7 +3135,7 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>665cbd19-b44d-44bf-84a7-31443c077891</t>
+          <t>522c5b16-c600-4928-a9f7-ab093decf3fd</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -3169,7 +3169,7 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>62e596ba-80ab-41a7-8b33-64afa566b040</t>
+          <t>bf4cce8c-3c54-4cdf-9fe8-6a65c0d5466e</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -3203,7 +3203,7 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>5bd1838a-9d1a-48f5-803f-2dbd4c9f9461</t>
+          <t>c54247db-b010-481f-aee2-6af6d08782ec</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -3237,7 +3237,7 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>67d3ea7d-08e9-4202-9c0b-6ce113e72fad</t>
+          <t>d3eb59aa-46e5-44ce-bde2-d1e3529cc5f9</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -3271,7 +3271,7 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>de459a89-a8ba-4ff5-a44c-3139ca46bdf3</t>
+          <t>aee18f6c-3a4c-44b1-99ac-768c933edaf1</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -3305,7 +3305,7 @@
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>696760eb-4c3e-493d-8355-5d6ff3335ce6</t>
+          <t>e627f395-9f19-4725-8dc4-8497c1724244</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -3339,7 +3339,7 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>2173168e-e02d-46d9-bc38-2eb852e07660</t>
+          <t>a37e3cf9-f44d-4d70-b3d1-a16edb7237c5</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -3373,7 +3373,7 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>d42635cc-981f-467a-af14-5de7c0918d07</t>
+          <t>8e115f00-fef7-4bca-8f57-ac9dbfe7cfcc</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -3407,7 +3407,7 @@
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>67f4d0ab-88d1-41bf-bf68-b247eb7b5cdb</t>
+          <t>bfbffe7d-79b3-47d2-82fa-80cee847a0c1</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -3441,7 +3441,7 @@
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>d44b5df1-8ff4-421c-8ea3-f51ce88ce747</t>
+          <t>3f511abb-bedf-4e13-8a6b-d9b9e335da41</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -3475,7 +3475,7 @@
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>052f74e8-945b-4a76-86fe-6adf67c28744</t>
+          <t>73730e2f-7ba6-40ae-9857-a13c64dfab9e</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -3509,7 +3509,7 @@
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>68f80441-ac40-4787-9661-330302abc76a</t>
+          <t>a35d1867-79df-45e2-895b-a37c62724dd3</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -3543,7 +3543,7 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>f94ea131-ccf7-4146-9dc0-c3d70e8e1821</t>
+          <t>75ac0199-b5c4-4247-a734-e48912762ef3</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -3577,7 +3577,7 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>da9297c1-ea4d-491b-98db-4df17c45350c</t>
+          <t>fa126f16-8c6e-4393-8b34-beb4591d32d4</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -3611,7 +3611,7 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>97aab9db-daff-473b-9d87-8e403588d2e5</t>
+          <t>f4ed18cd-b203-4e22-a57a-b538f0e2d58a</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -3645,7 +3645,7 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>9de03a82-4db4-448e-b9e6-976f7ae1802a</t>
+          <t>3d36282b-3ac7-412e-8123-661874737238</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -3679,7 +3679,7 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>111b7ddd-0595-4d52-931c-0abec7c58060</t>
+          <t>89090a52-3dbd-41a2-ba7a-804f51da0561</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -3713,7 +3713,7 @@
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>6285ec56-3fa5-4d25-8d88-ee48b24715d9</t>
+          <t>45c288dc-4c7e-4780-b15f-8d148d31eabd</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -3747,7 +3747,7 @@
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>3a7bf12d-e214-49c4-b2ca-09e5daaf5e3a</t>
+          <t>071a879b-a453-408f-98ff-38816330c73d</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -3781,7 +3781,7 @@
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>5035c3ef-9bfe-4378-a7e0-545903bc9d2e</t>
+          <t>72ca80dd-9243-4959-96e2-a887276c3c96</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -3815,7 +3815,7 @@
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>c4bef85f-1d23-4193-8d84-0bdb0ea3dc28</t>
+          <t>061f397c-be31-4d0f-977f-b43a87200484</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -3849,7 +3849,7 @@
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>516e602e-da29-4c2f-b2cf-d8a3ee27bf91</t>
+          <t>a90a8881-6b12-47b7-9df2-df9157b5f5da</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -3883,7 +3883,7 @@
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>82005b88-b908-4ab3-bb29-f12f68e643e8</t>
+          <t>f547ec92-f316-4227-a1a9-3d39bd8cea9e</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -3917,7 +3917,7 @@
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>940d45ba-c9e9-4f16-84d6-8f7fde689b36</t>
+          <t>26308baf-a842-4f1d-94e9-f177bd00fc7c</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -3951,7 +3951,7 @@
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>b9fd245b-af3c-4b1a-aafc-7b7e683cdb4c</t>
+          <t>7f0c9c64-50da-4041-ade0-e31f9b412929</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -3985,7 +3985,7 @@
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>89357a82-d307-4f34-b69b-715be1ae524f</t>
+          <t>d0c02d6c-8ebc-41aa-82b8-c4ef1ec2919c</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -4019,7 +4019,7 @@
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>078004f2-51df-4a4f-a0be-b4b7c3833fb6</t>
+          <t>ff5aabc5-00a9-45d7-a7e4-77fc23506ec2</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -4053,7 +4053,7 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>6c6cb14e-cfd7-4b7c-856c-d4162bc2319a</t>
+          <t>2f3b452b-833c-4ec4-8152-4d6f07efe22f</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -4087,7 +4087,7 @@
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>1fe245ba-884f-4b3a-8b99-282866247a2f</t>
+          <t>f927a03a-1df7-4c97-b926-117cbed815bd</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -4121,7 +4121,7 @@
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>ae26a365-7926-46ae-9874-607601c0ad82</t>
+          <t>f7d54625-574c-413a-b79a-5fe6e472e3cb</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -4155,7 +4155,7 @@
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>41261685-e508-482a-9a9e-f358a7a6db00</t>
+          <t>6399041d-445c-424e-a813-a99627813646</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -4189,7 +4189,7 @@
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>e77148a6-0b8a-4b50-b292-665f35976ae9</t>
+          <t>241e6b84-c711-48b1-898d-411c7e120c62</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -4223,7 +4223,7 @@
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>fbdbbf20-8374-4b9b-a36a-4c86ce767913</t>
+          <t>68edd4c2-db62-453a-9ea4-cd8a813b9299</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -4257,7 +4257,7 @@
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>dc7c5ba2-9788-464c-8eaf-8c6ee47ca876</t>
+          <t>072ee9fd-ba89-4596-9e2b-4abbba5dae22</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -4291,7 +4291,7 @@
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>ce8ccd7b-906d-4b6d-892d-2cc2be317ad6</t>
+          <t>015dda3a-3e3f-4f6d-8578-4cc53dd97930</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -4325,7 +4325,7 @@
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>feaa060d-5413-4e99-9e5e-a678a0cbec81</t>
+          <t>228d03b3-33e5-425f-b65a-4d4e692287e2</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -4359,7 +4359,7 @@
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>f6802e34-e932-41f1-94a8-abd30e8aa892</t>
+          <t>6de33224-3ad8-4df5-bbd0-5c3e15677cda</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -4393,7 +4393,7 @@
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>e367a80d-f384-4e81-b026-969a7d12921b</t>
+          <t>cf933199-7e0e-4678-b327-8b1483cd1492</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -4427,7 +4427,7 @@
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>af8b8fde-cd03-4ca1-998e-c910364555a5</t>
+          <t>ba18de72-27f9-4bd2-b80e-2377636feea2</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -4461,7 +4461,7 @@
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>688ffcaf-dbc0-46f4-9b83-bddc4f445b11</t>
+          <t>24c54c08-c3f4-494e-837c-297dd246eba6</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -4495,7 +4495,7 @@
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>ce0b0c5f-68b6-49d6-9b53-85f7e8d35f3f</t>
+          <t>74725281-1a9f-465a-bbfe-f986e8dc2864</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -4529,7 +4529,7 @@
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>c453c470-8244-47a1-a459-25755872e09f</t>
+          <t>af35b31c-04c9-4309-af8c-d87f9fd4c607</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -4563,7 +4563,7 @@
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>d27bc6c8-b01c-4c6c-a60f-e9b2625b86ab</t>
+          <t>e4e4f6ee-2eb2-4920-af79-8a7e9d9dd8af</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -4597,7 +4597,7 @@
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>d05ad22f-2142-47b0-abba-2bb328eac068</t>
+          <t>efa599b2-48ac-42af-af1f-ec9646847b58</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -4631,7 +4631,7 @@
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>3c82f150-1f4e-4fa3-a8fe-a06062f5e39c</t>
+          <t>b9420c55-0b2a-4749-a8e1-87f16db83c76</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -4665,7 +4665,7 @@
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>134aee8e-7adf-4663-97a3-50ccf28d2747</t>
+          <t>9e20fcc1-fbe1-4ff9-94d2-f100f17a59a2</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -4699,7 +4699,7 @@
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>ad1e662f-4bfe-499b-b388-b7e9763987ad</t>
+          <t>af467845-03c6-4eef-8be5-39f229224c97</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -4733,7 +4733,7 @@
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>e4f15d9e-725c-42e7-b1af-b891a5428313</t>
+          <t>7c5c7650-5e80-4418-a69f-9698a4efeda9</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -4767,7 +4767,7 @@
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>c61f6676-60a1-408d-86a5-c035284dd56f</t>
+          <t>41d260c5-0cde-4aab-b155-9f40b5cc3c25</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -4801,7 +4801,7 @@
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>33fc6397-9c61-4193-b0e0-a7509b81fbb9</t>
+          <t>d0b8c20b-6bf2-4415-a58e-21859e8d34ca</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -4835,7 +4835,7 @@
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>511a910d-383e-40dc-800e-814d2dad5e35</t>
+          <t>f960e644-c335-4cba-ac37-0c626adf179b</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -4869,7 +4869,7 @@
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>7522f8f7-5882-436a-b393-9924d5bb6001</t>
+          <t>47dbfb6a-01c5-4ebd-9b01-86d28f4f1f7b</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -4903,7 +4903,7 @@
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>a9171618-ea4e-4eb8-a56d-a4cc050f09d1</t>
+          <t>f835aed4-a7e6-4b2b-83d1-cca32ce2533e</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -4937,7 +4937,7 @@
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>d4cb0e99-e98d-4c59-a55f-12c971460186</t>
+          <t>2d23721b-198d-4230-a125-bafd159123a8</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -4971,7 +4971,7 @@
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>deef31a2-1430-454c-bd70-90eba564cb80</t>
+          <t>243d8825-d162-4fe8-ba8a-5a9c5d12ba1f</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -5005,7 +5005,7 @@
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>819a75a3-d07f-49ee-ba11-afee7421e735</t>
+          <t>5b48bd26-2f1c-4104-bfc8-a2f584802f23</t>
         </is>
       </c>
       <c r="B135" t="n">
@@ -5039,7 +5039,7 @@
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>4317c874-9e06-4161-80f9-0775043d5b4c</t>
+          <t>2004da9c-1179-4b4b-907c-da264fba2fb3</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -5073,7 +5073,7 @@
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>f34922f9-19cc-45db-b554-9ec3267fd5b2</t>
+          <t>8144a5ff-1e1e-4df8-815a-31c91be991f2</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -5107,7 +5107,7 @@
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>653f77df-9ffd-49bc-bac7-ca43df293084</t>
+          <t>d5f55a7a-7e14-48cf-86b5-ed6a58673d83</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -5141,7 +5141,7 @@
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>cb1a0ac3-9885-459f-8687-d67d308f0a8a</t>
+          <t>7a9f2879-8430-4932-97fa-99ab6f2ad6fc</t>
         </is>
       </c>
       <c r="B139" t="n">
@@ -5175,7 +5175,7 @@
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>b5e8a160-d79b-4946-adf8-5c87043c8eef</t>
+          <t>0cecf38e-c769-4b8f-a40d-cd34a91760ac</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -5209,7 +5209,7 @@
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>621c0961-5c89-452a-bb30-1bb35059277a</t>
+          <t>59ad4329-4467-4f00-9e16-6ff177868930</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -5243,7 +5243,7 @@
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>b64f8159-43e4-4241-8b40-1aa351796217</t>
+          <t>60afb06d-accd-4cd0-b1e7-c495d64646cc</t>
         </is>
       </c>
       <c r="B142" t="n">
@@ -5277,7 +5277,7 @@
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>7ab76df1-8552-46f7-a4d3-265d07cca087</t>
+          <t>9944e269-adf3-432c-bd91-b384b11e4815</t>
         </is>
       </c>
       <c r="B143" t="n">
@@ -5311,7 +5311,7 @@
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>3a824299-093d-4bb7-aec8-8732ea43ccd0</t>
+          <t>3de08b5b-83d1-44f4-ac79-dcbac196654e</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -5345,7 +5345,7 @@
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>91f9107a-95bd-4ae2-80ec-dae1b65c632b</t>
+          <t>97f22309-c7f1-4fd9-98b8-79a10cb59008</t>
         </is>
       </c>
       <c r="B145" t="n">
@@ -5379,7 +5379,7 @@
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>0bb85eb3-5a5c-4ec7-8204-51722112e2f7</t>
+          <t>e6352868-6765-4f81-9f4b-1b36e9c24e85</t>
         </is>
       </c>
       <c r="B146" t="n">
@@ -5413,7 +5413,7 @@
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>03cb2b31-0af7-4ba9-b577-8e9135e1ef11</t>
+          <t>c0a5f6e7-a8bb-4acb-8f27-68b3f7d4c677</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -5447,7 +5447,7 @@
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>426cd05c-a494-4528-85b9-d9ccca5c1c93</t>
+          <t>6d8237bb-8872-4571-8d6c-26e12d531444</t>
         </is>
       </c>
       <c r="B148" t="n">
@@ -5481,7 +5481,7 @@
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>bcd24066-79a0-4521-be4f-21e8cb7c4a80</t>
+          <t>adbfd73f-0b57-4966-95e7-d7f017d9c166</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -5515,7 +5515,7 @@
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
         <is>
-          <t>f86f9d83-98c6-415e-b264-27ed36783c3b</t>
+          <t>91d25ebc-2ce7-4ed6-8ddb-760be284fb2b</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -5549,7 +5549,7 @@
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>b1247f0c-6006-458a-b603-341b2055676b</t>
+          <t>c5468660-b3aa-4d9d-9008-00e8f19d614f</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -5583,7 +5583,7 @@
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>09fb438c-7068-475e-aa70-b0ba88e0c6b9</t>
+          <t>cb666cbb-ec06-418a-b584-d83914c822b2</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -5617,7 +5617,7 @@
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>bd600735-c41e-41c6-9162-61a4724d42ca</t>
+          <t>5ecfdd91-d57c-4a92-ae0d-6740415f7a37</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -5651,7 +5651,7 @@
     <row r="154">
       <c r="A154" s="1" t="inlineStr">
         <is>
-          <t>91121be3-e5c5-4f59-a16a-7e8a6e8454c0</t>
+          <t>f20e4e0c-f3fb-4aca-8c13-2b1690d9787e</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -5685,7 +5685,7 @@
     <row r="155">
       <c r="A155" s="1" t="inlineStr">
         <is>
-          <t>27bf8638-22ba-4638-98e6-d8a78d34ad7e</t>
+          <t>162dabe8-79a3-4c65-b6a6-83755f20a626</t>
         </is>
       </c>
       <c r="B155" t="n">
@@ -5719,7 +5719,7 @@
     <row r="156">
       <c r="A156" s="1" t="inlineStr">
         <is>
-          <t>3acd3df7-8fda-4035-8645-e30918c58ae7</t>
+          <t>2d2921ac-5b48-477c-8cff-7f86d864ef13</t>
         </is>
       </c>
       <c r="B156" t="n">
@@ -5753,7 +5753,7 @@
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
         <is>
-          <t>4fb58e38-6a83-4a66-9426-1cbf89d1af4c</t>
+          <t>9d576517-2b00-42aa-9676-abd03c748eab</t>
         </is>
       </c>
       <c r="B157" t="n">
@@ -5787,7 +5787,7 @@
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
-          <t>f3231c5b-1b75-47a7-9b0a-d195174086e6</t>
+          <t>fd3d0872-bdf0-439b-a153-147ddf3e4c66</t>
         </is>
       </c>
       <c r="B158" t="n">
@@ -5821,7 +5821,7 @@
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
-          <t>3d82f852-8a9f-4de9-8ac4-84c2d259b789</t>
+          <t>f75d57d2-ff1f-4ff4-8902-f22132c9f5c6</t>
         </is>
       </c>
       <c r="B159" t="n">
@@ -5855,7 +5855,7 @@
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
-          <t>2acf2d24-ab05-40cd-98ef-c25eefbbd6eb</t>
+          <t>d9dfe558-7d3f-45cf-b6a6-33bfcdbd4ff3</t>
         </is>
       </c>
       <c r="B160" t="n">
@@ -5889,7 +5889,7 @@
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>091f4c01-31cf-49cf-acbb-94df3fe5e45c</t>
+          <t>fb62edad-7a30-4013-bdc1-a9a30702aa67</t>
         </is>
       </c>
       <c r="B161" t="n">
@@ -5923,7 +5923,7 @@
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
         <is>
-          <t>75e1a527-9c82-4490-978d-5a0aa5b3ecab</t>
+          <t>ae0a82fe-c47e-46c5-a87c-2eec4bc7be96</t>
         </is>
       </c>
       <c r="B162" t="n">
@@ -5957,7 +5957,7 @@
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>86931b01-9942-422b-a401-d84a99383d22</t>
+          <t>cc5147e9-1b31-45f4-bd19-b8cd5cb5cc8d</t>
         </is>
       </c>
       <c r="B163" t="n">
@@ -5991,7 +5991,7 @@
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>e995243e-dcb9-4fd1-8c0c-b3e3883bb4b2</t>
+          <t>7fe146aa-7205-493b-8e98-a4103b2a1975</t>
         </is>
       </c>
       <c r="B164" t="n">
@@ -6025,7 +6025,7 @@
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>b8e0aafe-0fab-4ddd-a1b6-0e86ac13a405</t>
+          <t>77f74a87-e9f1-4056-8286-28777d818b76</t>
         </is>
       </c>
       <c r="B165" t="n">
@@ -6059,7 +6059,7 @@
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>41867d41-fbcc-4ff4-955e-38e98bb5fc10</t>
+          <t>7937c2dd-59f3-42ae-86d3-745eb72ed533</t>
         </is>
       </c>
       <c r="B166" t="n">
@@ -6093,7 +6093,7 @@
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>fb17da0f-7be1-431b-8fe7-a8179e78da9c</t>
+          <t>da1d3c5b-ec28-4152-a5ef-732cf5ae659c</t>
         </is>
       </c>
       <c r="B167" t="n">
@@ -6127,7 +6127,7 @@
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>54b36857-73ba-4f88-a15b-303cdc886b72</t>
+          <t>a9d56d32-4b97-410c-8650-35e0babd7cf2</t>
         </is>
       </c>
       <c r="B168" t="n">
@@ -6161,7 +6161,7 @@
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>dd3a1264-6fa8-4688-a49c-03a449720810</t>
+          <t>44235234-3c26-499e-9328-673c1df7a24a</t>
         </is>
       </c>
       <c r="B169" t="n">
@@ -6195,7 +6195,7 @@
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>8810505d-1bd2-48a1-817c-f8e3b17df3a5</t>
+          <t>a5f427c8-02f2-4801-9cfa-77fc0687ca39</t>
         </is>
       </c>
       <c r="B170" t="n">
@@ -6229,7 +6229,7 @@
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>bafed555-d58d-446f-b41a-ec16971142b0</t>
+          <t>f52e3a88-d292-4d33-ae89-392bf80925e0</t>
         </is>
       </c>
       <c r="B171" t="n">
@@ -6263,7 +6263,7 @@
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>6ed2bca0-ef43-4d80-a9a3-6749f9843a59</t>
+          <t>ebfd1779-980a-4961-b15c-db946a7fb54d</t>
         </is>
       </c>
       <c r="B172" t="n">
@@ -6297,7 +6297,7 @@
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>9bc24f6e-df1a-4fb9-a1fe-53178c6318c3</t>
+          <t>8e6ac83b-c91f-46fc-83ac-27eb7944908e</t>
         </is>
       </c>
       <c r="B173" t="n">
@@ -6331,7 +6331,7 @@
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>25f88c33-d185-4aea-9a8a-97f46d2b14e4</t>
+          <t>c782fd14-6c23-4ed5-a8ea-0dc4d4c0cbac</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -6365,7 +6365,7 @@
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>83334a4f-ae6a-4995-a0de-903303af9df2</t>
+          <t>2861624d-8ad5-4f6b-80df-12371ff0c704</t>
         </is>
       </c>
       <c r="B175" t="n">
@@ -6399,7 +6399,7 @@
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>3ebb97a0-32aa-49cb-9c83-c23b493ef25e</t>
+          <t>f3f3001c-6dec-4077-8ef1-cbe19cc4fb30</t>
         </is>
       </c>
       <c r="B176" t="n">
@@ -6433,7 +6433,7 @@
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>4f374a98-6b10-4c72-9cf3-279215e38819</t>
+          <t>32433c78-21cc-474e-a5fe-8cd568610276</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -6467,7 +6467,7 @@
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>a5a70fed-eda9-42ba-816b-ba7b1091224f</t>
+          <t>85ec6aee-d59b-415e-9488-d12e6b035817</t>
         </is>
       </c>
       <c r="B178" t="n">
@@ -6501,7 +6501,7 @@
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>1f718785-37d8-4908-892d-e09eb11b347f</t>
+          <t>0089c81a-d1e5-4377-9ed9-7fd94aae69c5</t>
         </is>
       </c>
       <c r="B179" t="n">
@@ -6535,7 +6535,7 @@
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>10367cf9-4814-4acb-a791-821b79bbc676</t>
+          <t>6b3383c7-a57a-4a7b-a29b-b1b090815792</t>
         </is>
       </c>
       <c r="B180" t="n">
@@ -6569,7 +6569,7 @@
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>2ae1f521-b196-4a38-81e0-11439c530ee3</t>
+          <t>e758cfd7-20ef-41be-96cd-eb2478661576</t>
         </is>
       </c>
       <c r="B181" t="n">
@@ -6603,7 +6603,7 @@
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>5f116028-7c60-4c21-8905-e8446814af38</t>
+          <t>7874b541-0c8a-4f7f-8eee-a3c23f0b9d5b</t>
         </is>
       </c>
       <c r="B182" t="n">
@@ -6637,7 +6637,7 @@
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>83df93f5-918d-4347-95a4-e609b8bb5d9d</t>
+          <t>b7107ec3-3043-4f87-9323-3967f81e8cd7</t>
         </is>
       </c>
       <c r="B183" t="n">
@@ -6671,7 +6671,7 @@
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>390cac68-25e4-4746-b851-673a15f4d327</t>
+          <t>43f045e7-919b-4e28-91ad-a91a9956b55a</t>
         </is>
       </c>
       <c r="B184" t="n">
@@ -6705,7 +6705,7 @@
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>7179af08-32d9-4722-a440-962b8a94e1d3</t>
+          <t>b6c551d2-18c9-4dba-a972-632290c53e31</t>
         </is>
       </c>
       <c r="B185" t="n">
@@ -6739,7 +6739,7 @@
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>8e77932d-3ea2-424b-a778-21aa67d5f59a</t>
+          <t>f6d81871-3362-41a3-b3ac-e57fd33af1c8</t>
         </is>
       </c>
       <c r="B186" t="n">
@@ -6773,7 +6773,7 @@
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>4508fb36-5e43-46d1-8781-15ff938c2ced</t>
+          <t>85533594-cccf-48e1-addc-623648a9bdc9</t>
         </is>
       </c>
       <c r="B187" t="n">
@@ -6807,7 +6807,7 @@
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>72344c91-e9bb-466a-9e87-a242f481030f</t>
+          <t>a22b3911-a69f-4d9e-b879-5a857c115595</t>
         </is>
       </c>
       <c r="B188" t="n">
@@ -6841,7 +6841,7 @@
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>f6dfcd7d-8aee-4bdc-acee-ea1e11c51232</t>
+          <t>20f217b9-030b-4555-bf6e-86ccfc6c2ce0</t>
         </is>
       </c>
       <c r="B189" t="n">
@@ -6875,7 +6875,7 @@
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>978ec210-7adc-4c15-a6ba-849cfbc4037e</t>
+          <t>701a0262-f3ef-4ee7-97dd-d7befc306a04</t>
         </is>
       </c>
       <c r="B190" t="n">
@@ -6909,7 +6909,7 @@
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>88706027-505d-44d5-a241-86dc0e73fffb</t>
+          <t>2c2d8bb3-78ab-4cf0-b18d-3f4adb46ca24</t>
         </is>
       </c>
       <c r="B191" t="n">
@@ -6943,7 +6943,7 @@
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>512148e7-887c-4913-be31-093260b4b393</t>
+          <t>54b0e82e-7ba4-4f22-9c30-69c9e6131117</t>
         </is>
       </c>
       <c r="B192" t="n">
@@ -6977,7 +6977,7 @@
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>cb78665e-96ca-42a0-b311-b27a63bc5987</t>
+          <t>07551728-f046-4769-8ac0-5eaa40179171</t>
         </is>
       </c>
       <c r="B193" t="n">
@@ -7011,7 +7011,7 @@
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>13fa62c9-a66e-4527-882d-48518b823f99</t>
+          <t>47488cd0-ea9d-40e4-8070-080563b8fa5d</t>
         </is>
       </c>
       <c r="B194" t="n">
@@ -7045,7 +7045,7 @@
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>09782cbe-24cd-40dc-b0e8-1e2c4a84e850</t>
+          <t>37816401-0624-448f-9141-ddd045878ab4</t>
         </is>
       </c>
       <c r="B195" t="n">
@@ -7079,7 +7079,7 @@
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>58011b70-38e0-4b48-a779-db06383e5f17</t>
+          <t>7fdd617a-570f-4f23-902a-7f4631d33e35</t>
         </is>
       </c>
       <c r="B196" t="n">
@@ -7113,7 +7113,7 @@
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>eb407710-2fbb-4720-a44e-a6b311c10d8e</t>
+          <t>7374dcc0-e7b7-4c0d-b474-d3aa4ea25813</t>
         </is>
       </c>
       <c r="B197" t="n">
@@ -7147,7 +7147,7 @@
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>eef7828e-8df5-48d0-b9d2-d0872472c17a</t>
+          <t>063e5b04-093f-4d99-bcaf-6c0e0088a786</t>
         </is>
       </c>
       <c r="B198" t="n">
@@ -7181,7 +7181,7 @@
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>d588a906-c579-41ba-b1d4-ba2c2bcf8ea5</t>
+          <t>034083a0-3a38-4a5c-b8d4-7698718fb9b4</t>
         </is>
       </c>
       <c r="B199" t="n">
@@ -7215,7 +7215,7 @@
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>be6b31c3-ea29-40c9-9c5c-37d10c742022</t>
+          <t>8b393cf7-51d7-4427-b1a3-407fdde59ff3</t>
         </is>
       </c>
       <c r="B200" t="n">
@@ -7249,7 +7249,7 @@
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>8bbe113f-ebd5-40e5-b4c8-309758acb30a</t>
+          <t>a90cf4f8-27d5-4e37-a45d-a1fc9ef59249</t>
         </is>
       </c>
       <c r="B201" t="n">
@@ -7283,7 +7283,7 @@
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>2ee844f9-7611-4577-90cf-3e651ebf2d07</t>
+          <t>114d0460-4ae2-4065-ae9d-f70c5c2262b8</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -7317,7 +7317,7 @@
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>2b7079e6-98e1-42d0-b2ab-2bbcaa2af4a4</t>
+          <t>b711eb24-0f41-42ca-99cd-3dda2d035141</t>
         </is>
       </c>
       <c r="B203" t="n">
@@ -7351,7 +7351,7 @@
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>be5204ab-712d-4b11-ba64-caf467a7d541</t>
+          <t>75a8d0a0-9e81-4781-b31f-99df90168baa</t>
         </is>
       </c>
       <c r="B204" t="n">
@@ -7385,7 +7385,7 @@
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>c1ad6d7e-2091-4068-bd83-92f38220a548</t>
+          <t>8e681635-1568-429c-9a54-6a6c1e295cb1</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -7419,7 +7419,7 @@
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>0ea5e869-fd1e-49f3-993c-34853c4ca52f</t>
+          <t>a2e7bbff-ed0c-42a7-8c4a-8aaf9804e249</t>
         </is>
       </c>
       <c r="B206" t="n">
@@ -7453,7 +7453,7 @@
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>c378dbf5-b75f-4632-9cae-d4c07cf850c7</t>
+          <t>49e56920-e393-4c60-abe7-3fb4f1b9b9fb</t>
         </is>
       </c>
       <c r="B207" t="n">
@@ -7487,7 +7487,7 @@
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>1d79fc51-f73e-41de-87db-d071ae49cdac</t>
+          <t>c3b6d44a-aab7-4144-9c6b-c08a512ace03</t>
         </is>
       </c>
       <c r="B208" t="n">
@@ -7521,7 +7521,7 @@
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>d557c815-a886-4d96-b25a-24f1cbf71408</t>
+          <t>32a7c5ed-42a2-4db0-9284-ae5411ae2142</t>
         </is>
       </c>
       <c r="B209" t="n">
@@ -7555,7 +7555,7 @@
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>6548493f-dc8d-4c27-b3d5-6e090f3bea4c</t>
+          <t>373f5139-2a7a-4410-92b9-7b535fc20541</t>
         </is>
       </c>
       <c r="B210" t="n">
@@ -7589,7 +7589,7 @@
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>727531e4-b772-41bd-9d91-0d21d2e560ed</t>
+          <t>776e03e2-16b0-4041-a011-6f824a3c43d9</t>
         </is>
       </c>
       <c r="B211" t="n">
@@ -7623,7 +7623,7 @@
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>9c876c48-a927-4602-9603-6bba597b1836</t>
+          <t>33a4d505-aac7-442a-a410-0ac3ecb9714c</t>
         </is>
       </c>
       <c r="B212" t="n">
@@ -7657,7 +7657,7 @@
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>23159151-66e9-4434-8b31-35ef8cc34780</t>
+          <t>39254bb5-4be8-4f22-ae24-62abbd37f425</t>
         </is>
       </c>
       <c r="B213" t="n">
@@ -7691,7 +7691,7 @@
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>2bf40567-79c6-4050-b5e5-dc001af50cf0</t>
+          <t>1d21edef-0c1c-4a17-9fcc-39e6d1cc759b</t>
         </is>
       </c>
       <c r="B214" t="n">
@@ -7725,7 +7725,7 @@
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>a7d7b10f-4012-4e8f-8438-2a6c4173b5f6</t>
+          <t>0944baf6-25be-493f-a430-854eca9e9fbe</t>
         </is>
       </c>
       <c r="B215" t="n">
@@ -7759,7 +7759,7 @@
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>7576be70-693c-4ebb-a31f-5057a40b6020</t>
+          <t>a703eee4-f63a-488f-9d91-2f14ed76331e</t>
         </is>
       </c>
       <c r="B216" t="n">
@@ -7793,7 +7793,7 @@
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>144712cf-a6d1-40e2-88d7-51499c1acbcc</t>
+          <t>f7a04df9-8ca2-4876-ae03-a7e7d6fe37a3</t>
         </is>
       </c>
       <c r="B217" t="n">
@@ -7827,7 +7827,7 @@
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>99dba985-7183-4e02-936e-7e803a4357f8</t>
+          <t>30aed096-b069-4a9d-a354-838295dbf43d</t>
         </is>
       </c>
       <c r="B218" t="n">
@@ -7861,7 +7861,7 @@
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>95d1e03a-e2b9-4e13-8130-a62ac80caa7f</t>
+          <t>3aa8b351-2c06-4b70-8a24-a5a3e2e4a2ab</t>
         </is>
       </c>
       <c r="B219" t="n">
@@ -7895,7 +7895,7 @@
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>72e7daa8-0ab4-4614-97e1-ba78a49337aa</t>
+          <t>7a47fa75-5c85-4fd9-994b-88ec6516d39d</t>
         </is>
       </c>
       <c r="B220" t="n">
@@ -7929,7 +7929,7 @@
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>b49e592b-cdca-40c0-885d-8593f2442643</t>
+          <t>50cbea65-a888-4a2b-ac25-9e37285e939b</t>
         </is>
       </c>
       <c r="B221" t="n">
@@ -7963,7 +7963,7 @@
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>2d0084c4-d5fe-445e-8440-46470cbdc21a</t>
+          <t>5e549784-41dd-4efd-bfa6-559a8d9850c5</t>
         </is>
       </c>
       <c r="B222" t="n">
@@ -7997,7 +7997,7 @@
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>b63c51fc-5b8f-447e-b9a0-39072e1f7794</t>
+          <t>90242b1a-612c-4eff-b96e-cc6a4958235d</t>
         </is>
       </c>
       <c r="B223" t="n">
@@ -8031,7 +8031,7 @@
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>a027faf0-ecab-49f4-9c32-6707c60ae848</t>
+          <t>ec7c074c-dc0d-40e3-ad7b-c00b264e553d</t>
         </is>
       </c>
       <c r="B224" t="n">
@@ -8065,7 +8065,7 @@
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>68c9266f-0ea0-429d-b0b9-7228382b82b0</t>
+          <t>9c5ae98f-4f89-457f-945b-377798c47a4d</t>
         </is>
       </c>
       <c r="B225" t="n">
@@ -8099,7 +8099,7 @@
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>ad25697f-3cbe-44ea-a20e-ead2e0ea2185</t>
+          <t>5c554bb0-5be7-4a9f-bbb3-eb50fb847d2c</t>
         </is>
       </c>
       <c r="B226" t="n">
@@ -8133,7 +8133,7 @@
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>889e6f64-abfa-4715-99b7-f28bc6d83da3</t>
+          <t>6885040c-46f5-42a7-9946-9aee2faff48f</t>
         </is>
       </c>
       <c r="B227" t="n">
@@ -8167,7 +8167,7 @@
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>b996efa2-be42-40e5-8d7b-c1a5d5d4e41c</t>
+          <t>706cf7a8-363e-45b6-97fa-b354e125c7b6</t>
         </is>
       </c>
       <c r="B228" t="n">
@@ -8201,7 +8201,7 @@
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>5a1da133-7569-4c61-8508-24234b1cffd1</t>
+          <t>690dbfad-78f2-422b-a342-0fb1cfb3979b</t>
         </is>
       </c>
       <c r="B229" t="n">
@@ -8235,7 +8235,7 @@
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>79e639fb-7a5f-4cfa-ae9c-0ec5dc76c886</t>
+          <t>fc9edca8-a243-45e6-a1b6-3b18f32aa9d2</t>
         </is>
       </c>
       <c r="B230" t="n">
@@ -8269,7 +8269,7 @@
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>45ec560a-eba5-4ec9-a0b9-c862df0fb588</t>
+          <t>ce25340b-e4ff-45f8-a586-5e11918924a5</t>
         </is>
       </c>
       <c r="B231" t="n">
@@ -8303,7 +8303,7 @@
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>8be32df7-6bfa-4b92-9c4f-31a780b4bac3</t>
+          <t>a114f91f-0759-4bf4-9df4-39bd00186c91</t>
         </is>
       </c>
       <c r="B232" t="n">
@@ -8337,7 +8337,7 @@
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>46f379be-08ff-4bc1-92a6-ce6827c2e688</t>
+          <t>7e4e51c6-8612-4a0d-8b01-2c5cc39f8a2f</t>
         </is>
       </c>
       <c r="B233" t="n">
@@ -8371,7 +8371,7 @@
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>765a6e2a-76ef-4819-8310-97b39ae8f266</t>
+          <t>aae941a3-3fac-4dd1-8cef-99cabefa878e</t>
         </is>
       </c>
       <c r="B234" t="n">
@@ -8405,7 +8405,7 @@
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>2f2a8982-0b40-4d72-a99b-44cc38395d81</t>
+          <t>751f7d9a-d623-4b3b-9909-ee775f073b85</t>
         </is>
       </c>
       <c r="B235" t="n">
@@ -8439,7 +8439,7 @@
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>1e56a542-591f-4928-b64d-36192c912a39</t>
+          <t>f372fe92-6781-4063-98f2-087fcfe78d6d</t>
         </is>
       </c>
       <c r="B236" t="n">
@@ -8473,7 +8473,7 @@
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>c2e6e46e-b18b-4c10-93c7-98439db06b2e</t>
+          <t>79978ad9-89cb-4227-814e-ef93fd9f3161</t>
         </is>
       </c>
       <c r="B237" t="n">
@@ -8507,7 +8507,7 @@
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>48f65f2e-3287-408c-ae14-1a3f79d91b09</t>
+          <t>ca6d11db-25af-4dab-b74a-60c656484780</t>
         </is>
       </c>
       <c r="B238" t="n">
@@ -8541,7 +8541,7 @@
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>26f97dfb-c8cb-4d02-9f18-dbd946025c76</t>
+          <t>b766724c-f4bc-4734-b351-0c4d832d917d</t>
         </is>
       </c>
       <c r="B239" t="n">
@@ -8575,7 +8575,7 @@
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>0a992d45-e301-4452-899a-2f016cecf67a</t>
+          <t>7661686b-7d4b-455d-81a8-8d3011e3d5f4</t>
         </is>
       </c>
       <c r="B240" t="n">
@@ -8609,7 +8609,7 @@
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>82be4744-0134-462b-aeb4-6ce54edb926f</t>
+          <t>416d469a-aea5-4797-be3d-731e7e6e6f9e</t>
         </is>
       </c>
       <c r="B241" t="n">
@@ -8643,7 +8643,7 @@
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>63f70e31-0ff9-4447-9016-25ab8f0a4e7c</t>
+          <t>2c64a6c9-9200-4bb8-b72b-89862f6d887d</t>
         </is>
       </c>
       <c r="B242" t="n">
@@ -8677,7 +8677,7 @@
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>1a40adba-d4b8-41ff-8ce4-e1f83f293120</t>
+          <t>4a089810-f90f-4356-aee2-46b0ad55f575</t>
         </is>
       </c>
       <c r="B243" t="n">
@@ -8711,7 +8711,7 @@
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>bd4abc74-f085-4a9e-8e10-9645262d5014</t>
+          <t>e81263e0-25a7-4de4-99de-bc312c240810</t>
         </is>
       </c>
       <c r="B244" t="n">
@@ -8745,7 +8745,7 @@
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>2b45a2d9-cfb2-4656-b8a2-1fdfae659f32</t>
+          <t>61fcfc0c-5280-487e-8cce-67e5308ee5a3</t>
         </is>
       </c>
       <c r="B245" t="n">
@@ -8779,7 +8779,7 @@
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>10a108ca-fe97-4444-a2f2-813c0b35e223</t>
+          <t>bc84376a-de7d-4168-b27f-88aef514e7a0</t>
         </is>
       </c>
       <c r="B246" t="n">
@@ -8813,7 +8813,7 @@
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>12d4252a-82dd-41c8-82ed-820ebeedfdb2</t>
+          <t>e74be12d-9381-4705-885c-a406a4603622</t>
         </is>
       </c>
       <c r="B247" t="n">
@@ -8847,7 +8847,7 @@
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>1e724ef5-ce98-4b46-8c7f-3706b805cd32</t>
+          <t>49d630af-7698-4a17-ab01-bc87d9ec85e1</t>
         </is>
       </c>
       <c r="B248" t="n">
@@ -8881,7 +8881,7 @@
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>dddcb496-e71c-442e-b209-995446c0aff3</t>
+          <t>fc0cb857-26a8-4865-84f5-1995ffd09e0e</t>
         </is>
       </c>
       <c r="B249" t="n">
@@ -8915,7 +8915,7 @@
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>fc22e8a4-262c-4249-a9b0-2f7344bbbb06</t>
+          <t>4923f583-a0dd-4183-ae8d-3c735b5da154</t>
         </is>
       </c>
       <c r="B250" t="n">
@@ -8949,7 +8949,7 @@
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>84469ac7-692b-41f4-b6d6-27d432cdb4fa</t>
+          <t>30bcbf8d-5e76-4ae9-8e34-7ee3ace7eea6</t>
         </is>
       </c>
       <c r="B251" t="n">
@@ -8983,7 +8983,7 @@
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>7858982e-4ca5-4512-8d07-651ccd931b1f</t>
+          <t>d1830155-8a96-48e9-b881-4b5f9a116265</t>
         </is>
       </c>
       <c r="B252" t="n">
@@ -9017,7 +9017,7 @@
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>1e3b88ce-2188-4845-88c0-b4624ce41db5</t>
+          <t>f7f63023-6696-4098-8691-f440a977647a</t>
         </is>
       </c>
       <c r="B253" t="n">
@@ -9051,7 +9051,7 @@
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>953edece-c6c3-4785-a0d4-737c01ccf14a</t>
+          <t>5895a50f-abf8-4bb2-8913-3022f41d8f6e</t>
         </is>
       </c>
       <c r="B254" t="n">
@@ -9085,7 +9085,7 @@
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>641bcc09-6fc5-4df7-87d9-4386dc608621</t>
+          <t>82472fc8-387f-4229-9b27-a5c69f0a30d2</t>
         </is>
       </c>
       <c r="B255" t="n">
@@ -9119,7 +9119,7 @@
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>4068c529-3616-4b72-9435-e056515a3abf</t>
+          <t>68e1c460-e55a-4abb-b2ba-1fc33d691374</t>
         </is>
       </c>
       <c r="B256" t="n">
@@ -9153,7 +9153,7 @@
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>4077cb61-256c-4d45-b56d-51edcf56ad11</t>
+          <t>0064e23d-02f6-4a9f-8d8d-d26280e61779</t>
         </is>
       </c>
       <c r="B257" t="n">
@@ -9187,7 +9187,7 @@
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>856edf0d-b252-4d63-964b-8f036d01ddcb</t>
+          <t>2d7cf89b-400d-47d9-a160-ff8628b68430</t>
         </is>
       </c>
       <c r="B258" t="n">
@@ -9221,7 +9221,7 @@
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>c5e78104-1481-40dc-af61-7a14457502f6</t>
+          <t>cdb9f7ef-3ac3-4163-8f25-7004d18d619f</t>
         </is>
       </c>
       <c r="B259" t="n">
@@ -9255,7 +9255,7 @@
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>aa12718a-d9f2-4f5e-a016-6a5bba02cdf4</t>
+          <t>355fc84f-94d4-4bde-9902-f45e4ccdb02d</t>
         </is>
       </c>
       <c r="B260" t="n">
@@ -9289,7 +9289,7 @@
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>a5b74c47-719b-4d3c-b241-95d123669ed7</t>
+          <t>576bf41c-aeee-4508-bf04-cb76a80e139f</t>
         </is>
       </c>
       <c r="B261" t="n">
@@ -9323,7 +9323,7 @@
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>e7a69f52-1477-4eb0-87fd-eb5b408c982d</t>
+          <t>26638997-f57f-4d3e-be1d-d815d556c276</t>
         </is>
       </c>
       <c r="B262" t="n">
@@ -9357,7 +9357,7 @@
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>5c17ae54-eba1-4d0d-90f1-d8136748f409</t>
+          <t>80099469-bce3-426b-8493-9be60bb728ba</t>
         </is>
       </c>
       <c r="B263" t="n">
@@ -9391,7 +9391,7 @@
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>45dc9fea-10bb-4959-a81f-9abed8d0bbab</t>
+          <t>4affb7a2-a6f3-48b4-b22c-ecc53b59a742</t>
         </is>
       </c>
       <c r="B264" t="n">
@@ -9425,7 +9425,7 @@
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>ac628a3b-ea27-4985-a080-6cc1883a34bd</t>
+          <t>ffd717ba-34f0-41ac-ae4b-1050c771fd01</t>
         </is>
       </c>
       <c r="B265" t="n">
@@ -9459,7 +9459,7 @@
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>cdc44c30-61e5-47b7-90c2-8662b03e30ee</t>
+          <t>dfcf5689-cf88-4939-99dc-c2889e9b3b44</t>
         </is>
       </c>
       <c r="B266" t="n">
@@ -9493,7 +9493,7 @@
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>d3ff5f19-17b1-4aa0-86e2-0c582e9bd89b</t>
+          <t>2555e90e-57f4-4731-99d6-133385513e18</t>
         </is>
       </c>
       <c r="B267" t="n">
@@ -9527,7 +9527,7 @@
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>99f3fd31-165d-4aca-aabb-e61d5b36c443</t>
+          <t>370eaf1f-4884-4305-96fe-c80807680555</t>
         </is>
       </c>
       <c r="B268" t="n">
@@ -9561,7 +9561,7 @@
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>24a58dd7-2d0a-4e48-8985-ee6f349026d8</t>
+          <t>a2efe789-2e3a-48e1-8fcf-f68aeb37c590</t>
         </is>
       </c>
       <c r="B269" t="n">
@@ -9595,7 +9595,7 @@
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>32006e32-40e5-4573-9293-35d395cfb3c2</t>
+          <t>cae67845-a584-494a-a503-d403740f651e</t>
         </is>
       </c>
       <c r="B270" t="n">
@@ -9629,7 +9629,7 @@
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>9c743ce2-8d1a-49b3-8e8f-e17a378b9033</t>
+          <t>34057d3f-19df-40ce-83b6-6e87cd540167</t>
         </is>
       </c>
       <c r="B271" t="n">
@@ -9663,7 +9663,7 @@
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>231a0d06-c16a-4154-a6c9-412803cdcf5b</t>
+          <t>e38aee2d-e97b-49cf-9471-3f4378317b0e</t>
         </is>
       </c>
       <c r="B272" t="n">
@@ -9697,7 +9697,7 @@
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>25ab7d62-fa04-4ef3-8520-1a0fda52c400</t>
+          <t>adad8528-0e81-40e9-9cbf-0132554b39c3</t>
         </is>
       </c>
       <c r="B273" t="n">
@@ -9731,7 +9731,7 @@
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>542aa7d2-83dc-48bd-921d-6ed9ddcec090</t>
+          <t>d547a32b-58ce-4e5f-9429-48166b4bf567</t>
         </is>
       </c>
       <c r="B274" t="n">
@@ -9765,7 +9765,7 @@
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>d63cfcf8-b20a-49f2-a781-0cbe0f769092</t>
+          <t>6bc4dbbc-f9f2-405b-aef3-a9eed6bd97e1</t>
         </is>
       </c>
       <c r="B275" t="n">
@@ -9799,7 +9799,7 @@
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>9f76b4f2-bc07-4c13-985a-885ce8921fae</t>
+          <t>2b5f791a-344c-4267-aaa8-f2ffe246b033</t>
         </is>
       </c>
       <c r="B276" t="n">
@@ -9833,7 +9833,7 @@
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>d60410f2-b883-4266-a63e-72b63aff8a9a</t>
+          <t>fc8ea102-268c-4da5-87ca-4feadce540cc</t>
         </is>
       </c>
       <c r="B277" t="n">
@@ -9867,7 +9867,7 @@
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>51d32a90-ce18-4d5d-afe3-ccaee9571065</t>
+          <t>61b005ae-473a-4941-9c7d-689200391f9b</t>
         </is>
       </c>
       <c r="B278" t="n">
@@ -9901,7 +9901,7 @@
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>8e12fc6e-717f-4b03-b0ec-a47e3474a968</t>
+          <t>9473d350-59ca-4ff0-a8a0-510aa5b11edc</t>
         </is>
       </c>
       <c r="B279" t="n">
@@ -9935,7 +9935,7 @@
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>5e4dd686-cf66-4fc0-8fa1-acfb66349783</t>
+          <t>b052303a-3833-4bec-9af3-5f135dd00a4e</t>
         </is>
       </c>
       <c r="B280" t="n">
@@ -9969,7 +9969,7 @@
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>fcf236a2-704a-4d14-ab90-fced8b259adc</t>
+          <t>90152e26-0095-4e63-8589-28fe960cf69b</t>
         </is>
       </c>
       <c r="B281" t="n">
@@ -10003,7 +10003,7 @@
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>582e9c42-84f8-4fe5-a33a-399a87a14f4c</t>
+          <t>e0bca826-2c26-4fb0-ab77-2764916a0ce1</t>
         </is>
       </c>
       <c r="B282" t="n">
@@ -10037,7 +10037,7 @@
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>461f5bc1-63e8-4ea3-aa82-dd9e62b557a1</t>
+          <t>ea8dc06f-9804-41ad-90b0-9a9a0fb55080</t>
         </is>
       </c>
       <c r="B283" t="n">
@@ -10071,7 +10071,7 @@
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>79908de0-d249-4dc1-9761-f57625b2ecb6</t>
+          <t>42237df5-843e-4c02-bd3f-bef27fa9243d</t>
         </is>
       </c>
       <c r="B284" t="n">
@@ -10105,7 +10105,7 @@
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>9bc18551-6485-4a59-9792-4165b24d859c</t>
+          <t>8074a800-52e1-4a44-8d1b-4b2c84fc9f65</t>
         </is>
       </c>
       <c r="B285" t="n">
@@ -10139,7 +10139,7 @@
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>dd29be63-3bb3-4671-95e0-5809b243ad10</t>
+          <t>70916cc3-1976-42e4-abbd-03fd88957399</t>
         </is>
       </c>
       <c r="B286" t="n">
@@ -10173,7 +10173,7 @@
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>db94217a-3f4d-40bd-95f5-19bbfb13e5a1</t>
+          <t>e4b919f4-4451-4312-9d43-91d8fcded4f9</t>
         </is>
       </c>
       <c r="B287" t="n">
@@ -10207,7 +10207,7 @@
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>fb3e5544-5da6-4ce1-a80b-95f60e86c358</t>
+          <t>3c66812c-f3d8-4394-a7d5-fdbc1d74aa82</t>
         </is>
       </c>
       <c r="B288" t="n">
@@ -10241,7 +10241,7 @@
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>53201d03-b05c-417a-a707-2badb7777aa3</t>
+          <t>91d2e18a-6204-4fba-8aa3-f487224b7563</t>
         </is>
       </c>
       <c r="B289" t="n">
@@ -10275,7 +10275,7 @@
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>f89c9fb5-7c3c-4e9c-a28e-e1d0389dade7</t>
+          <t>9ae82464-dd8e-4721-98be-c34056e647ba</t>
         </is>
       </c>
       <c r="B290" t="n">
@@ -10309,7 +10309,7 @@
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>58916c34-982c-42a3-824a-40931166976f</t>
+          <t>a8499d80-19ae-42ba-b201-de90c2db97f5</t>
         </is>
       </c>
       <c r="B291" t="n">
@@ -10343,7 +10343,7 @@
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>bc9d087d-1870-4b2e-8305-b749fecf0769</t>
+          <t>322a4c2a-5ab4-4646-be06-e732e8e49d25</t>
         </is>
       </c>
       <c r="B292" t="n">
@@ -10377,7 +10377,7 @@
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>75330355-7ae0-4549-ad12-3491c45f83f2</t>
+          <t>0c7c14a7-134c-4b77-8c52-4ee50c6f0d81</t>
         </is>
       </c>
       <c r="B293" t="n">
@@ -10411,7 +10411,7 @@
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>d3c9472d-de7e-4311-97f6-9af67a9c29a1</t>
+          <t>641ea9f2-5317-4ef4-badf-12989f830df9</t>
         </is>
       </c>
       <c r="B294" t="n">
@@ -10445,7 +10445,7 @@
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>cac7b117-aab8-4194-9040-e50fc35320ea</t>
+          <t>81214ad7-3fbc-4e87-b7f3-fb98d239565f</t>
         </is>
       </c>
       <c r="B295" t="n">
@@ -10479,7 +10479,7 @@
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>e529def7-1104-4ce2-8c8b-2ff9934d3839</t>
+          <t>8da5b3c8-bece-4fe4-be66-fae9c8d73a4b</t>
         </is>
       </c>
       <c r="B296" t="n">
@@ -10513,7 +10513,7 @@
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>94a3134e-2959-447a-b70f-ccd68be24249</t>
+          <t>c1b2ffd4-61d3-40fc-b570-3a1358e2bce6</t>
         </is>
       </c>
       <c r="B297" t="n">
@@ -10547,7 +10547,7 @@
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>6ef03abb-6a02-4a90-85ac-60c766852b5e</t>
+          <t>e3d49a0f-7483-445a-b368-5198392afadd</t>
         </is>
       </c>
       <c r="B298" t="n">
@@ -10581,7 +10581,7 @@
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>4195d8a4-47d0-4896-84b8-163fcc7152a4</t>
+          <t>7c0fd893-e70d-45e7-810b-29cb18841590</t>
         </is>
       </c>
       <c r="B299" t="n">
@@ -10615,7 +10615,7 @@
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>1147f68f-56b8-4f34-a6fa-21d47e4821c4</t>
+          <t>0d3ad800-120d-47b4-b473-4c1baa77a892</t>
         </is>
       </c>
       <c r="B300" t="n">
@@ -10649,7 +10649,7 @@
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>75779013-a2f7-4e63-8dd7-dd573f950c67</t>
+          <t>5a2d43ce-511d-4ace-87b9-9031dd7ce799</t>
         </is>
       </c>
       <c r="B301" t="n">
@@ -10683,7 +10683,7 @@
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>bd515bf9-241b-4cae-9b91-fd1d8587affe</t>
+          <t>bec2ebe2-3965-40f0-b9fe-de8669584f3a</t>
         </is>
       </c>
       <c r="B302" t="n">
@@ -10717,7 +10717,7 @@
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>76fc2e1c-28ae-4c50-9c21-52fce8cd0d2b</t>
+          <t>f2ce5aff-e81b-4c29-9701-9d95c128ef3e</t>
         </is>
       </c>
       <c r="B303" t="n">
@@ -10751,7 +10751,7 @@
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>622c223c-61f5-4a60-bc16-333bf33e2824</t>
+          <t>9b3645cd-a7fd-488b-ae2b-845712834b0a</t>
         </is>
       </c>
       <c r="B304" t="n">
@@ -10785,7 +10785,7 @@
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>6f94a448-e89e-4edd-ab42-ef72cfe6c361</t>
+          <t>46279122-4040-4376-b682-dee17fcfda20</t>
         </is>
       </c>
       <c r="B305" t="n">
@@ -10819,7 +10819,7 @@
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>c03d247b-e87c-44b2-a66a-7681d349c08f</t>
+          <t>5c8d0175-2462-4443-aaad-3f902c53532f</t>
         </is>
       </c>
       <c r="B306" t="n">
@@ -10853,7 +10853,7 @@
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>6f9aced8-7784-4d14-b487-10bc1e721cb0</t>
+          <t>55b380ee-696a-43e4-9fee-27eaab7bdf4c</t>
         </is>
       </c>
       <c r="B307" t="n">
@@ -10887,7 +10887,7 @@
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>49392ca8-2941-4a8d-bde6-e6c7b5f28fc0</t>
+          <t>cff32150-ca4c-4eaa-bd19-a0bae49ef616</t>
         </is>
       </c>
       <c r="B308" t="n">
@@ -10921,7 +10921,7 @@
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>a52db9d5-e7c3-4bc1-9716-207a7bba8e1e</t>
+          <t>3d2cc03b-63a9-4d81-ad24-4c0bce8fe0d9</t>
         </is>
       </c>
       <c r="B309" t="n">
@@ -10955,7 +10955,7 @@
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>90e74966-74f1-4afa-a8b3-e2e67d9094de</t>
+          <t>d53a1e62-2e82-432f-883c-a93662521bcc</t>
         </is>
       </c>
       <c r="B310" t="n">
@@ -10989,7 +10989,7 @@
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>4c2e8c89-695c-478c-a704-ddc4e53876da</t>
+          <t>d9f219b9-e58a-4871-aa35-57a1b788face</t>
         </is>
       </c>
       <c r="B311" t="n">
@@ -11023,7 +11023,7 @@
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>bf40f85e-458c-4112-b87d-bfaff8b66538</t>
+          <t>b193eb90-33ff-4b96-b64b-fdc830801b82</t>
         </is>
       </c>
       <c r="B312" t="n">
@@ -11057,7 +11057,7 @@
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>c5c26377-1a15-40ec-b927-80d43bf428bc</t>
+          <t>1b264581-410f-4957-8dcd-2da908cb7a2a</t>
         </is>
       </c>
       <c r="B313" t="n">
@@ -11091,7 +11091,7 @@
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>69d22f63-3196-4706-ab6c-947c730042a2</t>
+          <t>13dad48d-3d90-4417-9a4d-66d3def11deb</t>
         </is>
       </c>
       <c r="B314" t="n">
@@ -11125,7 +11125,7 @@
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>1e2112cf-fc52-4585-ad4c-5dcac1ac941c</t>
+          <t>e537e65b-3929-4e7d-a9af-81bad6c1040f</t>
         </is>
       </c>
       <c r="B315" t="n">
@@ -11159,7 +11159,7 @@
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>20cf9a80-99ec-410c-bc05-1c01d952fbce</t>
+          <t>fa004a0c-6f0f-4da1-858d-820da9c8dee2</t>
         </is>
       </c>
       <c r="B316" t="n">
@@ -11193,7 +11193,7 @@
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>8b408336-fcaf-4793-9ed7-271dc4106ef7</t>
+          <t>0b1c74f4-6c0f-4edf-aab9-71db8ab63c29</t>
         </is>
       </c>
       <c r="B317" t="n">
@@ -11227,7 +11227,7 @@
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>cdc127a0-7671-438d-8a70-547d49526060</t>
+          <t>7fc79d6e-2622-47e2-af98-cea23efb6036</t>
         </is>
       </c>
       <c r="B318" t="n">
@@ -11261,7 +11261,7 @@
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>76ecb5df-82d5-419f-a16c-3bbb6ccad06b</t>
+          <t>00f42a74-2dc9-4179-8d86-1b0b81d7600a</t>
         </is>
       </c>
       <c r="B319" t="n">
@@ -11295,7 +11295,7 @@
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>ea100516-681e-4dbe-90d6-561c83d97234</t>
+          <t>d1853485-0603-4be6-bf6c-f914a8ab18d4</t>
         </is>
       </c>
       <c r="B320" t="n">
@@ -11329,7 +11329,7 @@
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>bb0f6d57-9d2b-4a3a-994b-b4e9d6458162</t>
+          <t>4058cbcd-ef0b-49b7-b536-0026e320b69c</t>
         </is>
       </c>
       <c r="B321" t="n">
@@ -11363,7 +11363,7 @@
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>8bb2f9bb-7cb6-4dd2-8cc8-5d7379e13a32</t>
+          <t>55a278c3-ae16-475c-8903-0059391ec37f</t>
         </is>
       </c>
       <c r="B322" t="n">
@@ -11397,7 +11397,7 @@
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>92dcb63d-5e22-43e2-9d8e-4786b7384754</t>
+          <t>8350b040-0e84-4bc7-80fd-a672d289ca08</t>
         </is>
       </c>
       <c r="B323" t="n">
@@ -11431,7 +11431,7 @@
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>a497bbfc-ca1a-43a2-bc74-892a287682ea</t>
+          <t>92c7034c-db83-4191-8b85-1bbfae8f778a</t>
         </is>
       </c>
       <c r="B324" t="n">
@@ -11465,7 +11465,7 @@
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>4d7baa7b-fbfa-4c0d-80f1-bbd21bf35977</t>
+          <t>413dda8e-1cc6-4948-8daa-616e75f08776</t>
         </is>
       </c>
       <c r="B325" t="n">
@@ -11499,7 +11499,7 @@
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>d76869a5-a99c-4beb-b298-40dcb3f1b5d0</t>
+          <t>cb39e23a-8f19-4f57-92ba-af48fd7e7572</t>
         </is>
       </c>
       <c r="B326" t="n">
@@ -11533,7 +11533,7 @@
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>7dfbd793-a011-423a-a73f-1b61bb48ccc8</t>
+          <t>e75636c0-724a-4f8b-97cc-7f042fe97ed2</t>
         </is>
       </c>
       <c r="B327" t="n">
@@ -11567,7 +11567,7 @@
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>d042d007-1dcc-4172-a5c5-be72584e04ed</t>
+          <t>fdcc3460-8ca6-4803-9c30-de3ea8edc31c</t>
         </is>
       </c>
       <c r="B328" t="n">
@@ -11601,7 +11601,7 @@
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>b8eb60bd-82e7-4e23-8b45-fca02e32f0c7</t>
+          <t>c7de2075-788e-4bff-9142-2d2d2501941f</t>
         </is>
       </c>
       <c r="B329" t="n">
@@ -11635,7 +11635,7 @@
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
-          <t>90d530c1-079a-4393-b5f4-06076fb1b00a</t>
+          <t>c9ee3321-3cb3-4045-93a2-d39b4cc0a224</t>
         </is>
       </c>
       <c r="B330" t="n">
@@ -11669,7 +11669,7 @@
     <row r="331">
       <c r="A331" s="1" t="inlineStr">
         <is>
-          <t>a20b2781-39e7-4cc2-9bdc-8616458ef9b3</t>
+          <t>196bf487-288c-4b0a-8200-a5a947229da9</t>
         </is>
       </c>
       <c r="B331" t="n">
@@ -11703,7 +11703,7 @@
     <row r="332">
       <c r="A332" s="1" t="inlineStr">
         <is>
-          <t>351b9cd7-2108-403a-a860-46c7259a5de3</t>
+          <t>a5bdb06a-c5d7-4c9b-8045-a77a2ba5431b</t>
         </is>
       </c>
       <c r="B332" t="n">
@@ -11737,7 +11737,7 @@
     <row r="333">
       <c r="A333" s="1" t="inlineStr">
         <is>
-          <t>606a266a-8d24-440c-8193-06f2d501b453</t>
+          <t>330f3b9c-a7ef-40bd-a8e4-f18417fcf62e</t>
         </is>
       </c>
       <c r="B333" t="n">
@@ -11771,7 +11771,7 @@
     <row r="334">
       <c r="A334" s="1" t="inlineStr">
         <is>
-          <t>7d4762dc-448d-4879-98ec-630b76dde69c</t>
+          <t>c81aa98f-bd77-4119-999c-dd3d15b755a7</t>
         </is>
       </c>
       <c r="B334" t="n">
@@ -11805,7 +11805,7 @@
     <row r="335">
       <c r="A335" s="1" t="inlineStr">
         <is>
-          <t>e5af0737-6b4c-4491-93c4-2e330a50d821</t>
+          <t>2be2bfdf-34d8-4189-9151-5dee051ee800</t>
         </is>
       </c>
       <c r="B335" t="n">
@@ -11839,7 +11839,7 @@
     <row r="336">
       <c r="A336" s="1" t="inlineStr">
         <is>
-          <t>01f269fd-ab51-4bee-b6ce-1e142cbdba26</t>
+          <t>fbc9029a-a261-43fe-b708-a2f944d839f6</t>
         </is>
       </c>
       <c r="B336" t="n">
@@ -11873,7 +11873,7 @@
     <row r="337">
       <c r="A337" s="1" t="inlineStr">
         <is>
-          <t>6c9a61e9-a3d7-497f-9574-75d0f17e4d69</t>
+          <t>806f7524-f670-4bdc-894a-aa3e21b58c48</t>
         </is>
       </c>
       <c r="B337" t="n">
@@ -11907,7 +11907,7 @@
     <row r="338">
       <c r="A338" s="1" t="inlineStr">
         <is>
-          <t>6e4d2fbe-40b1-4bc9-a5d4-0f586fedfb64</t>
+          <t>47123c78-f71e-46b2-9a74-df23a340a350</t>
         </is>
       </c>
       <c r="B338" t="n">
@@ -11941,7 +11941,7 @@
     <row r="339">
       <c r="A339" s="1" t="inlineStr">
         <is>
-          <t>b10c9311-7d78-44a7-8c9c-171509f113cd</t>
+          <t>b3a4e046-823a-44ae-bb2b-b675b3b4a6e4</t>
         </is>
       </c>
       <c r="B339" t="n">
@@ -11975,7 +11975,7 @@
     <row r="340">
       <c r="A340" s="1" t="inlineStr">
         <is>
-          <t>fe48d1c7-d092-4186-b947-3a11ca75f6ca</t>
+          <t>66c0761f-6ea4-4808-8b50-7bd81d534d27</t>
         </is>
       </c>
       <c r="B340" t="n">
@@ -12009,7 +12009,7 @@
     <row r="341">
       <c r="A341" s="1" t="inlineStr">
         <is>
-          <t>ab32dd49-229b-4177-a1f0-13c62399797c</t>
+          <t>3ed3b643-a5dd-441a-bf2a-56b3192b2497</t>
         </is>
       </c>
       <c r="B341" t="n">
@@ -12043,7 +12043,7 @@
     <row r="342">
       <c r="A342" s="1" t="inlineStr">
         <is>
-          <t>39711b68-4281-4ef1-8409-7685bb763bd8</t>
+          <t>4c26d0a5-cca6-4949-b3ff-56f8effa8bf3</t>
         </is>
       </c>
       <c r="B342" t="n">
@@ -12077,7 +12077,7 @@
     <row r="343">
       <c r="A343" s="1" t="inlineStr">
         <is>
-          <t>9387c8c2-16ec-47af-a920-cf76eb8973c5</t>
+          <t>4c4e0cd9-5eae-4394-b50d-7e9db83439f5</t>
         </is>
       </c>
       <c r="B343" t="n">
@@ -12111,7 +12111,7 @@
     <row r="344">
       <c r="A344" s="1" t="inlineStr">
         <is>
-          <t>c362380d-02e0-4dad-a278-fb48b5bdf58d</t>
+          <t>11776cd9-0865-4d05-b36a-e88a33d55b07</t>
         </is>
       </c>
       <c r="B344" t="n">
@@ -12145,7 +12145,7 @@
     <row r="345">
       <c r="A345" s="1" t="inlineStr">
         <is>
-          <t>ba7d524a-e322-4d45-a7f5-69b87ca7275d</t>
+          <t>a8341886-f833-4429-b494-c4fb7d41dc0d</t>
         </is>
       </c>
       <c r="B345" t="n">
@@ -12179,7 +12179,7 @@
     <row r="346">
       <c r="A346" s="1" t="inlineStr">
         <is>
-          <t>fdff674d-d4ac-46b8-bfef-d1684d26e176</t>
+          <t>57b623ff-49c6-41d7-a340-6806622f9689</t>
         </is>
       </c>
       <c r="B346" t="n">
@@ -12213,7 +12213,7 @@
     <row r="347">
       <c r="A347" s="1" t="inlineStr">
         <is>
-          <t>c10e13c8-a2ad-4d4c-9c55-cc8c1fa0e31a</t>
+          <t>cd6034d2-c34d-4cdf-85fe-75e6bc580643</t>
         </is>
       </c>
       <c r="B347" t="n">
@@ -12247,7 +12247,7 @@
     <row r="348">
       <c r="A348" s="1" t="inlineStr">
         <is>
-          <t>3dbc9331-f04d-43fd-b6e7-51bf13ba33a3</t>
+          <t>08d1f9f5-5fbc-4aba-8e92-a91b157b23c9</t>
         </is>
       </c>
       <c r="B348" t="n">
@@ -12281,7 +12281,7 @@
     <row r="349">
       <c r="A349" s="1" t="inlineStr">
         <is>
-          <t>2e5a3cc0-5208-452e-84b6-557f7c89c864</t>
+          <t>9665d80a-d512-4516-9288-10e7e33fd50e</t>
         </is>
       </c>
       <c r="B349" t="n">
@@ -12315,7 +12315,7 @@
     <row r="350">
       <c r="A350" s="1" t="inlineStr">
         <is>
-          <t>6226b681-ddab-4af1-be54-edfb39c4197c</t>
+          <t>96cd61ca-f3d8-4429-8c1c-d8e8357fac9a</t>
         </is>
       </c>
       <c r="B350" t="n">
@@ -12349,7 +12349,7 @@
     <row r="351">
       <c r="A351" s="1" t="inlineStr">
         <is>
-          <t>d2a76e04-d162-416c-938c-2ff2b4e51d2d</t>
+          <t>3e67318f-7370-4d22-828c-96fcc0afe97d</t>
         </is>
       </c>
       <c r="B351" t="n">
@@ -12383,7 +12383,7 @@
     <row r="352">
       <c r="A352" s="1" t="inlineStr">
         <is>
-          <t>f4edd07b-6585-4d30-9de5-d9abc05d96bb</t>
+          <t>68f6fc61-41ca-48fd-907a-1098ca1eebbc</t>
         </is>
       </c>
       <c r="B352" t="n">
@@ -12417,7 +12417,7 @@
     <row r="353">
       <c r="A353" s="1" t="inlineStr">
         <is>
-          <t>50552073-61f5-4d90-9613-26047ee52900</t>
+          <t>88a0f011-f4ec-4a38-b6ee-b219d4c43dec</t>
         </is>
       </c>
       <c r="B353" t="n">
@@ -12451,7 +12451,7 @@
     <row r="354">
       <c r="A354" s="1" t="inlineStr">
         <is>
-          <t>9d1b8f3f-09ad-4381-9ce7-4e6268456f5c</t>
+          <t>42ba09d3-f9b3-4b82-b4d9-8aa9121c5ea6</t>
         </is>
       </c>
       <c r="B354" t="n">
@@ -12485,7 +12485,7 @@
     <row r="355">
       <c r="A355" s="1" t="inlineStr">
         <is>
-          <t>5c54ba75-11cb-4f73-898e-87746c00cf5c</t>
+          <t>02fc3d39-e668-40fb-a79b-36e556abec75</t>
         </is>
       </c>
       <c r="B355" t="n">
@@ -12519,7 +12519,7 @@
     <row r="356">
       <c r="A356" s="1" t="inlineStr">
         <is>
-          <t>766aec7f-104b-4cac-a85f-29efe1156fef</t>
+          <t>102ba6c6-1937-49b2-831d-b437607353d7</t>
         </is>
       </c>
       <c r="B356" t="n">
@@ -12553,7 +12553,7 @@
     <row r="357">
       <c r="A357" s="1" t="inlineStr">
         <is>
-          <t>bd323876-5ddd-4b2a-a4c8-ab0d87c70798</t>
+          <t>f304d7da-a8ce-470c-836b-a45a917c6b8c</t>
         </is>
       </c>
       <c r="B357" t="n">
@@ -12587,7 +12587,7 @@
     <row r="358">
       <c r="A358" s="1" t="inlineStr">
         <is>
-          <t>c3fd329e-8045-4984-8d67-1264a2deb77f</t>
+          <t>b905e7c8-c20d-403a-ab9e-9b777010f013</t>
         </is>
       </c>
       <c r="B358" t="n">
@@ -12621,7 +12621,7 @@
     <row r="359">
       <c r="A359" s="1" t="inlineStr">
         <is>
-          <t>01150c56-6ec8-4898-bb49-b6b2a2ee8b5b</t>
+          <t>57c4a1e9-8aec-47d8-9992-146b93bc90b2</t>
         </is>
       </c>
       <c r="B359" t="n">
@@ -12655,7 +12655,7 @@
     <row r="360">
       <c r="A360" s="1" t="inlineStr">
         <is>
-          <t>ff05b164-0873-4da2-a48a-f54dcfe98feb</t>
+          <t>ec41ca95-2f1c-43fb-bd8d-c452179f0cf3</t>
         </is>
       </c>
       <c r="B360" t="n">
@@ -12689,7 +12689,7 @@
     <row r="361">
       <c r="A361" s="1" t="inlineStr">
         <is>
-          <t>0c053130-a72f-4420-b3c6-08bd023c5021</t>
+          <t>2e7586fe-c1d9-40a4-a35f-3cb670883b22</t>
         </is>
       </c>
       <c r="B361" t="n">
@@ -12723,7 +12723,7 @@
     <row r="362">
       <c r="A362" s="1" t="inlineStr">
         <is>
-          <t>4bfa0f11-712d-4fca-8906-c6f31c26c2c9</t>
+          <t>39e72978-aaf4-4e42-ac30-9bc8e69a2ebe</t>
         </is>
       </c>
       <c r="B362" t="n">
@@ -12757,7 +12757,7 @@
     <row r="363">
       <c r="A363" s="1" t="inlineStr">
         <is>
-          <t>fecce054-dad5-4f0b-85ff-99cd26a3c45b</t>
+          <t>779f5a7e-6006-4cad-9be6-64ada1dc34bf</t>
         </is>
       </c>
       <c r="B363" t="n">
@@ -12791,7 +12791,7 @@
     <row r="364">
       <c r="A364" s="1" t="inlineStr">
         <is>
-          <t>cbb1cc2b-fae8-46fa-ac8b-f928acaaa62c</t>
+          <t>667ae6de-eb87-4856-8969-80dfef69dbee</t>
         </is>
       </c>
       <c r="B364" t="n">
@@ -12825,7 +12825,7 @@
     <row r="365">
       <c r="A365" s="1" t="inlineStr">
         <is>
-          <t>e680add2-ebe7-4ab6-a025-813d754365b2</t>
+          <t>efa4bac1-9de6-46d9-a534-65053e140003</t>
         </is>
       </c>
       <c r="B365" t="n">
@@ -12859,7 +12859,7 @@
     <row r="366">
       <c r="A366" s="1" t="inlineStr">
         <is>
-          <t>0edc1e0f-67a2-459e-86f1-599140bfeb37</t>
+          <t>cf4dec28-86b5-45c5-8eb6-c1662cb37eca</t>
         </is>
       </c>
       <c r="B366" t="n">
@@ -12893,7 +12893,7 @@
     <row r="367">
       <c r="A367" s="1" t="inlineStr">
         <is>
-          <t>bd6f38a9-3fcf-4a9e-8878-7e30a12865a8</t>
+          <t>211717b7-c2d7-4438-92b3-dc68a4de08f8</t>
         </is>
       </c>
       <c r="B367" t="n">
@@ -12927,7 +12927,7 @@
     <row r="368">
       <c r="A368" s="1" t="inlineStr">
         <is>
-          <t>191cbba1-4b14-4452-b16f-372fb23ed1de</t>
+          <t>b09534ff-a864-44ed-a797-2466b7d275f3</t>
         </is>
       </c>
       <c r="B368" t="n">
@@ -12961,7 +12961,7 @@
     <row r="369">
       <c r="A369" s="1" t="inlineStr">
         <is>
-          <t>af71d68a-6fab-48d3-81bd-4067d408f5f9</t>
+          <t>600bcc9b-34e4-4d22-8190-9a10fe16e0e6</t>
         </is>
       </c>
       <c r="B369" t="n">
@@ -12995,7 +12995,7 @@
     <row r="370">
       <c r="A370" s="1" t="inlineStr">
         <is>
-          <t>f71b6eb5-fe61-423a-9aaf-495a201709f5</t>
+          <t>322d4145-c74e-4ac5-a2a4-94f236c20ee4</t>
         </is>
       </c>
       <c r="B370" t="n">
@@ -13029,7 +13029,7 @@
     <row r="371">
       <c r="A371" s="1" t="inlineStr">
         <is>
-          <t>ec4dea50-7e36-4feb-a4dd-8173672d455a</t>
+          <t>3145cdc0-59a1-4673-bffa-a6affacd4b95</t>
         </is>
       </c>
       <c r="B371" t="n">
@@ -13063,7 +13063,7 @@
     <row r="372">
       <c r="A372" s="1" t="inlineStr">
         <is>
-          <t>f8c5ef1f-9c1c-4b20-b07c-7ced46fc9d93</t>
+          <t>1bb6d68d-11d9-44a0-8b79-e244b62eaaa6</t>
         </is>
       </c>
       <c r="B372" t="n">
@@ -13097,7 +13097,7 @@
     <row r="373">
       <c r="A373" s="1" t="inlineStr">
         <is>
-          <t>056d5006-b2da-4605-8ab7-246347b096de</t>
+          <t>1792fd1e-0bd2-44e9-b9fd-2afb5d38220a</t>
         </is>
       </c>
       <c r="B373" t="n">
@@ -13131,7 +13131,7 @@
     <row r="374">
       <c r="A374" s="1" t="inlineStr">
         <is>
-          <t>a28ce93a-e6b6-4ee9-aade-7f0a2c67c378</t>
+          <t>41e59525-7f25-4d2d-9512-3c858b7cbdcd</t>
         </is>
       </c>
       <c r="B374" t="n">
@@ -13165,7 +13165,7 @@
     <row r="375">
       <c r="A375" s="1" t="inlineStr">
         <is>
-          <t>215f17aa-fae5-4103-89d0-1ce29b2800d0</t>
+          <t>e2c1e8de-df9d-46d9-b289-89d591de57f5</t>
         </is>
       </c>
       <c r="B375" t="n">
@@ -13199,7 +13199,7 @@
     <row r="376">
       <c r="A376" s="1" t="inlineStr">
         <is>
-          <t>78b583cb-052d-4399-aeb2-a11e38b6a772</t>
+          <t>ef45f209-f5be-4f82-a759-1aa40e5f4389</t>
         </is>
       </c>
       <c r="B376" t="n">
@@ -13233,7 +13233,7 @@
     <row r="377">
       <c r="A377" s="1" t="inlineStr">
         <is>
-          <t>bb76480e-2f29-45bb-8a00-f39928228e89</t>
+          <t>98dc9fa2-72e4-41f4-a5a5-ffa5796d2005</t>
         </is>
       </c>
       <c r="B377" t="n">
@@ -13267,7 +13267,7 @@
     <row r="378">
       <c r="A378" s="1" t="inlineStr">
         <is>
-          <t>75aa431a-56ea-4a55-bca3-bfad47dee7a8</t>
+          <t>d525deca-39f7-4a7c-802a-5d912cd36ca0</t>
         </is>
       </c>
       <c r="B378" t="n">
@@ -13301,7 +13301,7 @@
     <row r="379">
       <c r="A379" s="1" t="inlineStr">
         <is>
-          <t>473acd13-57fc-40ec-97ed-1a5a3ebb9613</t>
+          <t>caee0904-1da1-4cd0-a538-a09af7e53674</t>
         </is>
       </c>
       <c r="B379" t="n">
@@ -13335,7 +13335,7 @@
     <row r="380">
       <c r="A380" s="1" t="inlineStr">
         <is>
-          <t>ba8b9ed1-d288-41a9-b664-e09f7a924d2e</t>
+          <t>572ae660-01be-4333-a2e9-da80406a19ff</t>
         </is>
       </c>
       <c r="B380" t="n">
@@ -13369,7 +13369,7 @@
     <row r="381">
       <c r="A381" s="1" t="inlineStr">
         <is>
-          <t>17bb5028-6aa3-4746-ae3f-bb3e7d468afc</t>
+          <t>fdc49974-5122-47d5-900e-4f3ff9177b47</t>
         </is>
       </c>
       <c r="B381" t="n">
@@ -13403,7 +13403,7 @@
     <row r="382">
       <c r="A382" s="1" t="inlineStr">
         <is>
-          <t>30944608-9a8c-46b6-9453-1aa10ccdcf75</t>
+          <t>53a91c67-d095-4d53-ada9-f677f0ad5187</t>
         </is>
       </c>
       <c r="B382" t="n">
@@ -13437,7 +13437,7 @@
     <row r="383">
       <c r="A383" s="1" t="inlineStr">
         <is>
-          <t>3581681b-578f-448d-ae3a-05d57b7e7a55</t>
+          <t>9d157d48-cc70-4b72-b71a-72452f8a1824</t>
         </is>
       </c>
       <c r="B383" t="n">
@@ -13471,7 +13471,7 @@
     <row r="384">
       <c r="A384" s="1" t="inlineStr">
         <is>
-          <t>6ce429ef-47ca-42ac-9dc9-391004f3429a</t>
+          <t>6c840784-7b59-4e2c-b20b-86a1bdee16d2</t>
         </is>
       </c>
       <c r="B384" t="n">
@@ -13505,7 +13505,7 @@
     <row r="385">
       <c r="A385" s="1" t="inlineStr">
         <is>
-          <t>a1582c6e-9d99-4dff-9d44-c31f5bfd8443</t>
+          <t>99998235-d990-4b22-9e24-70759c2fc156</t>
         </is>
       </c>
       <c r="B385" t="n">
@@ -13539,7 +13539,7 @@
     <row r="386">
       <c r="A386" s="1" t="inlineStr">
         <is>
-          <t>43ae324b-d6ac-4d91-a552-53d7072161e1</t>
+          <t>c827c1f8-acb7-4fa9-9b57-f4917aa6c4a0</t>
         </is>
       </c>
       <c r="B386" t="n">
@@ -13573,7 +13573,7 @@
     <row r="387">
       <c r="A387" s="1" t="inlineStr">
         <is>
-          <t>834f93ef-0f1c-4462-92c3-c05e4c62e055</t>
+          <t>6cf56e1d-2c13-44cc-b67c-b48338df451c</t>
         </is>
       </c>
       <c r="B387" t="n">
@@ -13607,7 +13607,7 @@
     <row r="388">
       <c r="A388" s="1" t="inlineStr">
         <is>
-          <t>85ae7471-61b0-406d-bd93-bf7bd4780d3a</t>
+          <t>688c4109-1474-4061-ad09-1f47698b3f09</t>
         </is>
       </c>
       <c r="B388" t="n">
@@ -13641,7 +13641,7 @@
     <row r="389">
       <c r="A389" s="1" t="inlineStr">
         <is>
-          <t>323ecc0c-d50b-42cf-a564-cd99e247d0a9</t>
+          <t>3b50bbed-91cd-4bb1-803d-7df99007aa97</t>
         </is>
       </c>
       <c r="B389" t="n">
@@ -13675,7 +13675,7 @@
     <row r="390">
       <c r="A390" s="1" t="inlineStr">
         <is>
-          <t>c0b2b981-3a72-4211-bddb-edea1f9cc0f0</t>
+          <t>b54a85a3-4624-42b0-a632-ee90a38d2c98</t>
         </is>
       </c>
       <c r="B390" t="n">
@@ -13709,7 +13709,7 @@
     <row r="391">
       <c r="A391" s="1" t="inlineStr">
         <is>
-          <t>dfb65fa7-0e02-47c7-b2b8-1525561dd046</t>
+          <t>588ac8a7-8ea9-44ef-b4e2-be636dd56198</t>
         </is>
       </c>
       <c r="B391" t="n">
@@ -13743,7 +13743,7 @@
     <row r="392">
       <c r="A392" s="1" t="inlineStr">
         <is>
-          <t>4102aeca-e8fd-4593-a847-91548c8d36c9</t>
+          <t>f2ea8d8e-de8a-40f0-a082-bfa5d6500ce6</t>
         </is>
       </c>
       <c r="B392" t="n">
@@ -13777,7 +13777,7 @@
     <row r="393">
       <c r="A393" s="1" t="inlineStr">
         <is>
-          <t>451d31c1-d7f0-422e-9ded-86f65ad8fe06</t>
+          <t>efacb1cc-8db8-45d2-988b-446cf58ffe1a</t>
         </is>
       </c>
       <c r="B393" t="n">
@@ -13811,7 +13811,7 @@
     <row r="394">
       <c r="A394" s="1" t="inlineStr">
         <is>
-          <t>469bf0f9-2fe2-42aa-a7a8-ddc8bce8cca9</t>
+          <t>c1d3fcab-96ce-4178-906d-ee47fde80244</t>
         </is>
       </c>
       <c r="B394" t="n">
@@ -13845,7 +13845,7 @@
     <row r="395">
       <c r="A395" s="1" t="inlineStr">
         <is>
-          <t>d8da7627-3e25-417f-b1ae-78350c3a403d</t>
+          <t>3e1943fa-2cd9-4fd8-8d00-e0d6cc76a0d4</t>
         </is>
       </c>
       <c r="B395" t="n">
@@ -13879,7 +13879,7 @@
     <row r="396">
       <c r="A396" s="1" t="inlineStr">
         <is>
-          <t>7cf0dae3-5111-4574-abfd-9738e60bc04d</t>
+          <t>9dee4f41-e69f-4264-9b59-1c76bf23a5d1</t>
         </is>
       </c>
       <c r="B396" t="n">
@@ -13913,7 +13913,7 @@
     <row r="397">
       <c r="A397" s="1" t="inlineStr">
         <is>
-          <t>f1b07413-a7fe-4a88-8c58-df64f34e5e7d</t>
+          <t>1967e3b3-46df-48b2-a06a-9483e21e1e4f</t>
         </is>
       </c>
       <c r="B397" t="n">
@@ -13947,7 +13947,7 @@
     <row r="398">
       <c r="A398" s="1" t="inlineStr">
         <is>
-          <t>05fc118b-415a-4255-8793-db00a18352b9</t>
+          <t>24e4c69d-5c90-49da-852d-b720b41f8cff</t>
         </is>
       </c>
       <c r="B398" t="n">
@@ -13981,7 +13981,7 @@
     <row r="399">
       <c r="A399" s="1" t="inlineStr">
         <is>
-          <t>ed4edf2b-f158-4af1-8b84-af04b76e8a29</t>
+          <t>33d72214-31fc-499a-8e51-b7fe7ffe25c4</t>
         </is>
       </c>
       <c r="B399" t="n">
@@ -14015,7 +14015,7 @@
     <row r="400">
       <c r="A400" s="1" t="inlineStr">
         <is>
-          <t>ff9ad9be-5543-42eb-87d7-30c3354fbad8</t>
+          <t>9150e65a-981d-4841-b59e-211609eb6663</t>
         </is>
       </c>
       <c r="B400" t="n">
@@ -14049,7 +14049,7 @@
     <row r="401">
       <c r="A401" s="1" t="inlineStr">
         <is>
-          <t>d5cfe9c7-dcd8-4311-97ab-ffd41b7798ee</t>
+          <t>3280c49c-5cc4-46e7-a7cf-3729578725aa</t>
         </is>
       </c>
       <c r="B401" t="n">
@@ -14083,7 +14083,7 @@
     <row r="402">
       <c r="A402" s="1" t="inlineStr">
         <is>
-          <t>adbf6e4c-57f6-4165-ba7c-987ec7c3b09b</t>
+          <t>d74303ce-c9a7-4f69-ab40-3561e8df9cc1</t>
         </is>
       </c>
       <c r="B402" t="n">
@@ -14117,7 +14117,7 @@
     <row r="403">
       <c r="A403" s="1" t="inlineStr">
         <is>
-          <t>886ce88c-9c74-421d-972f-320560974585</t>
+          <t>fe0b2456-0043-4290-ab17-295ea900c40e</t>
         </is>
       </c>
       <c r="B403" t="n">
@@ -14151,7 +14151,7 @@
     <row r="404">
       <c r="A404" s="1" t="inlineStr">
         <is>
-          <t>c543efc3-8129-4c88-8dee-3511b21cbda9</t>
+          <t>7e0a8a24-8867-44f1-b8e2-9585028a287b</t>
         </is>
       </c>
       <c r="B404" t="n">
@@ -14185,7 +14185,7 @@
     <row r="405">
       <c r="A405" s="1" t="inlineStr">
         <is>
-          <t>7e963f9c-0124-4999-b9bc-d293a9a23fba</t>
+          <t>1ee27205-2928-4fbc-ad8e-4f109d063626</t>
         </is>
       </c>
       <c r="B405" t="n">
@@ -14219,7 +14219,7 @@
     <row r="406">
       <c r="A406" s="1" t="inlineStr">
         <is>
-          <t>2562196c-d823-438f-8514-ba69bc640c51</t>
+          <t>de8f29e9-67d7-4b9a-9b2e-656e8bb46046</t>
         </is>
       </c>
       <c r="B406" t="n">
@@ -14253,7 +14253,7 @@
     <row r="407">
       <c r="A407" s="1" t="inlineStr">
         <is>
-          <t>88cfc3be-deb8-4e8a-8f5a-814eca847ffe</t>
+          <t>3ec8e3bf-7508-4b5f-adde-5eb4605ac971</t>
         </is>
       </c>
       <c r="B407" t="n">
@@ -14287,7 +14287,7 @@
     <row r="408">
       <c r="A408" s="1" t="inlineStr">
         <is>
-          <t>4e389653-ccbd-415f-9a18-85254a0d0814</t>
+          <t>bcb88514-e8b9-4a00-a233-987d4bebd04d</t>
         </is>
       </c>
       <c r="B408" t="n">
@@ -14321,7 +14321,7 @@
     <row r="409">
       <c r="A409" s="1" t="inlineStr">
         <is>
-          <t>ff9b62da-582c-4253-be06-13e26a236c1e</t>
+          <t>b1b027de-e4f0-4d26-acbe-4aec3b7ad244</t>
         </is>
       </c>
       <c r="B409" t="n">
@@ -14355,7 +14355,7 @@
     <row r="410">
       <c r="A410" s="1" t="inlineStr">
         <is>
-          <t>f2cd381d-3177-4cf6-afbc-5852fb5d3224</t>
+          <t>116edf13-4435-4c6c-9ccf-f27ca043f190</t>
         </is>
       </c>
       <c r="B410" t="n">
@@ -14389,7 +14389,7 @@
     <row r="411">
       <c r="A411" s="1" t="inlineStr">
         <is>
-          <t>685c5312-6006-42cc-a2a1-b698c5a23117</t>
+          <t>7ab1027d-3d39-4e07-87bc-0cd733ac22f2</t>
         </is>
       </c>
       <c r="B411" t="n">
@@ -14423,7 +14423,7 @@
     <row r="412">
       <c r="A412" s="1" t="inlineStr">
         <is>
-          <t>d65303a3-d711-4d3e-a2fd-9ae4da417784</t>
+          <t>68cafc44-70fb-4d6d-9b46-ffaeeec8cdc2</t>
         </is>
       </c>
       <c r="B412" t="n">
@@ -14457,7 +14457,7 @@
     <row r="413">
       <c r="A413" s="1" t="inlineStr">
         <is>
-          <t>d934e4d8-889f-4ac9-b964-19a60b5d04b0</t>
+          <t>8eaf680d-4534-4c6b-acbe-e0ed2beb6865</t>
         </is>
       </c>
       <c r="B413" t="n">
@@ -14491,7 +14491,7 @@
     <row r="414">
       <c r="A414" s="1" t="inlineStr">
         <is>
-          <t>893ec3fe-318a-4245-b624-b8c8edfbde15</t>
+          <t>c68f4466-11cb-494a-af02-ae0d5234d901</t>
         </is>
       </c>
       <c r="B414" t="n">
@@ -14525,7 +14525,7 @@
     <row r="415">
       <c r="A415" s="1" t="inlineStr">
         <is>
-          <t>6b206dda-da96-475e-bf21-3bacc7e6724f</t>
+          <t>6d2ac7cc-f637-4373-ab4e-1c3dc7264411</t>
         </is>
       </c>
       <c r="B415" t="n">
@@ -14559,7 +14559,7 @@
     <row r="416">
       <c r="A416" s="1" t="inlineStr">
         <is>
-          <t>3ac03963-b30e-431c-a89a-d0926dbf0017</t>
+          <t>02252eb4-c16a-4122-8c21-22d767767fbe</t>
         </is>
       </c>
       <c r="B416" t="n">
@@ -14593,7 +14593,7 @@
     <row r="417">
       <c r="A417" s="1" t="inlineStr">
         <is>
-          <t>f8b842b1-f74c-40ab-a283-7e15e09927d7</t>
+          <t>193b1b10-7444-4782-a396-e5e26fa05b38</t>
         </is>
       </c>
       <c r="B417" t="n">
@@ -14627,7 +14627,7 @@
     <row r="418">
       <c r="A418" s="1" t="inlineStr">
         <is>
-          <t>120230d8-4cfb-4e46-9960-56705b1e67fa</t>
+          <t>daceae00-d445-4e03-bc46-f6d1920937f4</t>
         </is>
       </c>
       <c r="B418" t="n">
@@ -14661,7 +14661,7 @@
     <row r="419">
       <c r="A419" s="1" t="inlineStr">
         <is>
-          <t>76872504-b69e-4e1d-8f4d-9840f3d2d057</t>
+          <t>17399521-ab4d-46cc-ac4f-20c22324e4fb</t>
         </is>
       </c>
       <c r="B419" t="n">
@@ -14695,7 +14695,7 @@
     <row r="420">
       <c r="A420" s="1" t="inlineStr">
         <is>
-          <t>22e0ee3a-3433-452a-be3d-66af4d6815b8</t>
+          <t>00be5a8e-bb32-45b6-9c37-c26e5a020dbb</t>
         </is>
       </c>
       <c r="B420" t="n">
@@ -14729,7 +14729,7 @@
     <row r="421">
       <c r="A421" s="1" t="inlineStr">
         <is>
-          <t>2bfe8717-0745-4c6a-b05d-58c3e8de2d8d</t>
+          <t>42b92517-76ff-4ddb-a320-93a707ef33a2</t>
         </is>
       </c>
       <c r="B421" t="n">
@@ -14763,7 +14763,7 @@
     <row r="422">
       <c r="A422" s="1" t="inlineStr">
         <is>
-          <t>38e9b8da-47c8-4597-a70e-f4fb1ed46ea1</t>
+          <t>c12b126d-8e62-45f3-beb8-8d26aa0f9bdb</t>
         </is>
       </c>
       <c r="B422" t="n">
@@ -14797,7 +14797,7 @@
     <row r="423">
       <c r="A423" s="1" t="inlineStr">
         <is>
-          <t>c31bcf59-9b67-47fe-b591-7f0203b0a0ff</t>
+          <t>ff27c5d3-53a9-4906-b618-b83dfeb9de94</t>
         </is>
       </c>
       <c r="B423" t="n">
@@ -14831,7 +14831,7 @@
     <row r="424">
       <c r="A424" s="1" t="inlineStr">
         <is>
-          <t>889c3852-568f-4667-98cb-773ef64a4876</t>
+          <t>1a96be71-94ca-4523-996f-e3c5f9ee126a</t>
         </is>
       </c>
       <c r="B424" t="n">
@@ -14865,7 +14865,7 @@
     <row r="425">
       <c r="A425" s="1" t="inlineStr">
         <is>
-          <t>b22d7d00-6f92-4f6b-ab43-2802c34fb7d2</t>
+          <t>f669dfd2-d4ac-4e46-9df4-73efcafae025</t>
         </is>
       </c>
       <c r="B425" t="n">
@@ -14899,7 +14899,7 @@
     <row r="426">
       <c r="A426" s="1" t="inlineStr">
         <is>
-          <t>a9f88247-9035-4291-832b-ba6763286b66</t>
+          <t>9fa01b2e-6f2c-4443-aed2-49c5722d2c9c</t>
         </is>
       </c>
       <c r="B426" t="n">
@@ -14933,7 +14933,7 @@
     <row r="427">
       <c r="A427" s="1" t="inlineStr">
         <is>
-          <t>31f8d8ab-2704-464d-8f8f-27a14a044b01</t>
+          <t>49877a98-c55c-49b7-841c-7efff1e1115c</t>
         </is>
       </c>
       <c r="B427" t="n">
@@ -14967,7 +14967,7 @@
     <row r="428">
       <c r="A428" s="1" t="inlineStr">
         <is>
-          <t>4db5dc93-6235-41d6-aade-22f39a1094f7</t>
+          <t>dbbdb501-4f1b-472c-a21c-3031c65ba549</t>
         </is>
       </c>
       <c r="B428" t="n">
@@ -15001,7 +15001,7 @@
     <row r="429">
       <c r="A429" s="1" t="inlineStr">
         <is>
-          <t>65169718-e7b1-48d8-bd93-c24257e308c0</t>
+          <t>9bacaf84-5fdb-45ab-97d2-d9a571ac0477</t>
         </is>
       </c>
       <c r="B429" t="n">
@@ -15035,7 +15035,7 @@
     <row r="430">
       <c r="A430" s="1" t="inlineStr">
         <is>
-          <t>19345375-b3f9-44f4-8255-4002c7600100</t>
+          <t>624c79cd-90b8-4aa6-b8e6-182ceecbccee</t>
         </is>
       </c>
       <c r="B430" t="n">
@@ -15069,7 +15069,7 @@
     <row r="431">
       <c r="A431" s="1" t="inlineStr">
         <is>
-          <t>35c63820-4c8e-4b45-a00d-6b3ed70400e2</t>
+          <t>f58c87b9-d084-4c1f-84e9-fa42390a6e67</t>
         </is>
       </c>
       <c r="B431" t="n">
@@ -15103,7 +15103,7 @@
     <row r="432">
       <c r="A432" s="1" t="inlineStr">
         <is>
-          <t>8decd096-4b29-4547-aa42-8d78c39ae454</t>
+          <t>983096f8-44cc-40a5-8f0e-51e0b423b120</t>
         </is>
       </c>
       <c r="B432" t="n">
@@ -15137,7 +15137,7 @@
     <row r="433">
       <c r="A433" s="1" t="inlineStr">
         <is>
-          <t>ce8f16ee-f26c-40ba-a938-89cf659984c0</t>
+          <t>f3a8bd8a-2ed5-4aee-8afa-fc4b2a7edd08</t>
         </is>
       </c>
       <c r="B433" t="n">
@@ -15171,7 +15171,7 @@
     <row r="434">
       <c r="A434" s="1" t="inlineStr">
         <is>
-          <t>84a65268-fb35-4af6-9207-6539766530f1</t>
+          <t>a78b071c-fbff-48c6-87c9-8c9cf7d29be0</t>
         </is>
       </c>
       <c r="B434" t="n">
@@ -15205,7 +15205,7 @@
     <row r="435">
       <c r="A435" s="1" t="inlineStr">
         <is>
-          <t>9db3e778-4a7a-4ff2-b1e0-e2acc9ab33c0</t>
+          <t>89a8651b-8b8a-4ca5-b74b-60e5d8c48468</t>
         </is>
       </c>
       <c r="B435" t="n">
@@ -15239,7 +15239,7 @@
     <row r="436">
       <c r="A436" s="1" t="inlineStr">
         <is>
-          <t>0feaeb9f-1ca9-46d1-8ade-f822387a90ba</t>
+          <t>82df82ce-df16-4407-879e-d0de5bdf236d</t>
         </is>
       </c>
       <c r="B436" t="n">
@@ -15273,7 +15273,7 @@
     <row r="437">
       <c r="A437" s="1" t="inlineStr">
         <is>
-          <t>af2d0450-93fb-4a3f-8552-050b3a19ae3c</t>
+          <t>8b1c6c6d-323c-4737-b3c9-4aab8a5a0899</t>
         </is>
       </c>
       <c r="B437" t="n">
@@ -15307,7 +15307,7 @@
     <row r="438">
       <c r="A438" s="1" t="inlineStr">
         <is>
-          <t>b0edee42-4c5d-4091-968f-3acc38c03ac5</t>
+          <t>8879bd08-ae75-477d-a185-0b6ef3de3fb7</t>
         </is>
       </c>
       <c r="B438" t="n">
@@ -15341,7 +15341,7 @@
     <row r="439">
       <c r="A439" s="1" t="inlineStr">
         <is>
-          <t>ba337a0b-c901-4c27-af5c-35a074ca2279</t>
+          <t>69d87ae5-3bef-47bc-bec2-2c370e3fe1a3</t>
         </is>
       </c>
       <c r="B439" t="n">
@@ -15375,7 +15375,7 @@
     <row r="440">
       <c r="A440" s="1" t="inlineStr">
         <is>
-          <t>e608a263-84d8-4e52-aa37-7562a15a6c66</t>
+          <t>a23816ba-a65c-472c-b90f-cbf1bf8a428d</t>
         </is>
       </c>
       <c r="B440" t="n">
@@ -15409,7 +15409,7 @@
     <row r="441">
       <c r="A441" s="1" t="inlineStr">
         <is>
-          <t>205c5a5f-eabb-452e-9c96-6e44c622703e</t>
+          <t>ec499944-6f36-43ef-acb9-72951a16f601</t>
         </is>
       </c>
       <c r="B441" t="n">
@@ -15443,7 +15443,7 @@
     <row r="442">
       <c r="A442" s="1" t="inlineStr">
         <is>
-          <t>893b61a2-5c02-44aa-b2ff-5c35d5b70bcf</t>
+          <t>eeb6947c-9fa5-4039-b11c-4015334d10b2</t>
         </is>
       </c>
       <c r="B442" t="n">
@@ -15477,7 +15477,7 @@
     <row r="443">
       <c r="A443" s="1" t="inlineStr">
         <is>
-          <t>8a7dfec8-8fc3-480c-859f-852d7784e22a</t>
+          <t>20b4f4b9-f85d-4a0f-8851-49a3f18cd4e3</t>
         </is>
       </c>
       <c r="B443" t="n">
@@ -15511,7 +15511,7 @@
     <row r="444">
       <c r="A444" s="1" t="inlineStr">
         <is>
-          <t>4de9fd6f-767c-4db6-b2f9-e615f4b11efa</t>
+          <t>9b566d70-3da0-480b-9651-dc439a4bf6b5</t>
         </is>
       </c>
       <c r="B444" t="n">
@@ -15545,7 +15545,7 @@
     <row r="445">
       <c r="A445" s="1" t="inlineStr">
         <is>
-          <t>d4f5675d-9737-4a0b-84b9-bfbd38eca0e2</t>
+          <t>0436fd12-53cf-4ae7-a6f3-e61ba048df65</t>
         </is>
       </c>
       <c r="B445" t="n">
@@ -15579,7 +15579,7 @@
     <row r="446">
       <c r="A446" s="1" t="inlineStr">
         <is>
-          <t>9bfba3df-2fb0-4000-9053-d89367202a4b</t>
+          <t>2eb98e29-acca-4910-a2ac-e43f0f695743</t>
         </is>
       </c>
       <c r="B446" t="n">
@@ -15613,7 +15613,7 @@
     <row r="447">
       <c r="A447" s="1" t="inlineStr">
         <is>
-          <t>80815903-9830-4d7d-b3fd-05d010e3ff15</t>
+          <t>4c1e6070-e363-4c7e-b005-e93e88b4dd6f</t>
         </is>
       </c>
       <c r="B447" t="n">
@@ -15647,7 +15647,7 @@
     <row r="448">
       <c r="A448" s="1" t="inlineStr">
         <is>
-          <t>c88dc75e-17e9-4cfb-919d-47f696666b78</t>
+          <t>a2d5c09f-2975-49f0-9b7b-036d998e4daa</t>
         </is>
       </c>
       <c r="B448" t="n">
@@ -15681,7 +15681,7 @@
     <row r="449">
       <c r="A449" s="1" t="inlineStr">
         <is>
-          <t>c58740d5-59a7-4c71-9521-d1eee35d82a3</t>
+          <t>406e2ced-32d9-4845-ac92-dac56b13a3a1</t>
         </is>
       </c>
       <c r="B449" t="n">
@@ -15715,7 +15715,7 @@
     <row r="450">
       <c r="A450" s="1" t="inlineStr">
         <is>
-          <t>a3212593-0105-479e-9048-fcc28b5dcce6</t>
+          <t>82dfb4ce-ce30-43cc-8fe6-0da2021b4a93</t>
         </is>
       </c>
       <c r="B450" t="n">
@@ -15749,7 +15749,7 @@
     <row r="451">
       <c r="A451" s="1" t="inlineStr">
         <is>
-          <t>9061a816-8f0c-408f-a955-90928f8a93e5</t>
+          <t>ad556b1e-4c8b-4649-951d-569fd3e9027a</t>
         </is>
       </c>
       <c r="B451" t="n">
@@ -15783,7 +15783,7 @@
     <row r="452">
       <c r="A452" s="1" t="inlineStr">
         <is>
-          <t>d6b54580-2d46-4b7e-b030-33d9c13c7081</t>
+          <t>89ba0424-6764-446e-b114-56c6a56c9973</t>
         </is>
       </c>
       <c r="B452" t="n">
@@ -15817,7 +15817,7 @@
     <row r="453">
       <c r="A453" s="1" t="inlineStr">
         <is>
-          <t>6114e116-e776-40b2-b217-86d3d6bbbe53</t>
+          <t>cd38ceda-66a0-4108-8d2a-60e2b0bf401b</t>
         </is>
       </c>
       <c r="B453" t="n">
@@ -15851,7 +15851,7 @@
     <row r="454">
       <c r="A454" s="1" t="inlineStr">
         <is>
-          <t>450ba625-742d-46c8-8466-bf8b5a15bbb1</t>
+          <t>abd2cbb8-b4a0-47cb-b046-b8ed87c59292</t>
         </is>
       </c>
       <c r="B454" t="n">
@@ -15885,7 +15885,7 @@
     <row r="455">
       <c r="A455" s="1" t="inlineStr">
         <is>
-          <t>628d3c6d-db81-44b3-a5bd-459f680d5497</t>
+          <t>6f396940-3486-4902-912a-3961c610997d</t>
         </is>
       </c>
       <c r="B455" t="n">
@@ -15919,7 +15919,7 @@
     <row r="456">
       <c r="A456" s="1" t="inlineStr">
         <is>
-          <t>221644ec-4161-46e3-9c00-99f09be822fb</t>
+          <t>12ac9a87-215f-489b-bec4-4a62a4ead612</t>
         </is>
       </c>
       <c r="B456" t="n">
@@ -15953,7 +15953,7 @@
     <row r="457">
       <c r="A457" s="1" t="inlineStr">
         <is>
-          <t>49cf958d-737f-423b-8f73-a57db3ed1322</t>
+          <t>e3cf4fae-3f34-4ddc-9257-54e819d3b22a</t>
         </is>
       </c>
       <c r="B457" t="n">
@@ -15987,7 +15987,7 @@
     <row r="458">
       <c r="A458" s="1" t="inlineStr">
         <is>
-          <t>b146cff7-0b05-4b29-a8cf-765f3c5851ea</t>
+          <t>b2dd7762-3db4-425f-92e1-b2ec877c247a</t>
         </is>
       </c>
       <c r="B458" t="n">
@@ -16021,7 +16021,7 @@
     <row r="459">
       <c r="A459" s="1" t="inlineStr">
         <is>
-          <t>1c11413c-6131-443c-8997-b9d096935f66</t>
+          <t>3a084273-5ac7-4816-bf9c-7f7f9d98e353</t>
         </is>
       </c>
       <c r="B459" t="n">
@@ -16055,7 +16055,7 @@
     <row r="460">
       <c r="A460" s="1" t="inlineStr">
         <is>
-          <t>01a13380-56af-4fa8-93c2-4ae4a9c63e49</t>
+          <t>b7a94750-153d-4730-8ca9-5803a4e77c76</t>
         </is>
       </c>
       <c r="B460" t="n">
@@ -16089,7 +16089,7 @@
     <row r="461">
       <c r="A461" s="1" t="inlineStr">
         <is>
-          <t>8ba64e7d-603f-4463-b42f-963586499164</t>
+          <t>2a95ed00-7edb-4157-a167-06990770db46</t>
         </is>
       </c>
       <c r="B461" t="n">
@@ -16123,7 +16123,7 @@
     <row r="462">
       <c r="A462" s="1" t="inlineStr">
         <is>
-          <t>9773fcbe-0f3f-46be-a1fb-da93f0cb96b6</t>
+          <t>ba93ac7a-a0c8-47b2-a941-df4d8e763e21</t>
         </is>
       </c>
       <c r="B462" t="n">
@@ -16157,7 +16157,7 @@
     <row r="463">
       <c r="A463" s="1" t="inlineStr">
         <is>
-          <t>f8a612cd-32c0-485b-8ce0-df1d8972e94b</t>
+          <t>06c14921-83b8-4bd7-b268-6044ab55ad25</t>
         </is>
       </c>
       <c r="B463" t="n">
@@ -16191,7 +16191,7 @@
     <row r="464">
       <c r="A464" s="1" t="inlineStr">
         <is>
-          <t>37d2624d-752a-4c68-9972-a50c0a40d82c</t>
+          <t>5a8a809a-198a-421b-940f-dbf96cc38771</t>
         </is>
       </c>
       <c r="B464" t="n">
@@ -16225,7 +16225,7 @@
     <row r="465">
       <c r="A465" s="1" t="inlineStr">
         <is>
-          <t>d8b61fef-00e5-42b0-afc9-cddf923c16e7</t>
+          <t>b4b66c98-a596-4805-aeeb-fd1bfd6a1090</t>
         </is>
       </c>
       <c r="B465" t="n">
@@ -16259,7 +16259,7 @@
     <row r="466">
       <c r="A466" s="1" t="inlineStr">
         <is>
-          <t>8659c505-0a0e-4a50-8b35-458840699603</t>
+          <t>f9abdfb9-35c3-41b4-b553-30a4d1d6ca92</t>
         </is>
       </c>
       <c r="B466" t="n">
@@ -16293,7 +16293,7 @@
     <row r="467">
       <c r="A467" s="1" t="inlineStr">
         <is>
-          <t>94e15dd1-9845-47ee-a527-069c44797782</t>
+          <t>6ee7a872-66db-4122-953a-ce2e2d70e768</t>
         </is>
       </c>
       <c r="B467" t="n">
@@ -16327,7 +16327,7 @@
     <row r="468">
       <c r="A468" s="1" t="inlineStr">
         <is>
-          <t>75b262d3-9504-40ae-bc4f-61f13b7d476f</t>
+          <t>d69f57ed-112a-4af2-b996-ef41cf014961</t>
         </is>
       </c>
       <c r="B468" t="n">
@@ -16361,7 +16361,7 @@
     <row r="469">
       <c r="A469" s="1" t="inlineStr">
         <is>
-          <t>58d72279-bee9-4a85-b204-63c877cf8547</t>
+          <t>42d694de-432b-4620-9ae2-54bff971c5bd</t>
         </is>
       </c>
       <c r="B469" t="n">
@@ -16395,7 +16395,7 @@
     <row r="470">
       <c r="A470" s="1" t="inlineStr">
         <is>
-          <t>41c07641-a038-4ab1-9360-3932e9d7f7ec</t>
+          <t>be4c3f6c-4040-4dda-8b23-6172c931446c</t>
         </is>
       </c>
       <c r="B470" t="n">
@@ -16429,7 +16429,7 @@
     <row r="471">
       <c r="A471" s="1" t="inlineStr">
         <is>
-          <t>ae75a996-2e6e-4005-9023-8b4c21624dbe</t>
+          <t>b2c15b11-5e2a-457b-bad5-0974d05f7276</t>
         </is>
       </c>
       <c r="B471" t="n">
@@ -16463,7 +16463,7 @@
     <row r="472">
       <c r="A472" s="1" t="inlineStr">
         <is>
-          <t>02a35390-1aca-4b99-b0d3-f196de413286</t>
+          <t>9262a15f-692e-4d84-91a3-b7200b4b1f89</t>
         </is>
       </c>
       <c r="B472" t="n">
@@ -16497,7 +16497,7 @@
     <row r="473">
       <c r="A473" s="1" t="inlineStr">
         <is>
-          <t>72289aca-93de-4c1e-afc7-c815b972b826</t>
+          <t>998b3a10-d79e-4bbf-8a72-6bc3ba75f73e</t>
         </is>
       </c>
       <c r="B473" t="n">
@@ -16531,7 +16531,7 @@
     <row r="474">
       <c r="A474" s="1" t="inlineStr">
         <is>
-          <t>09fcbe8d-23e3-4b39-b406-80aeaac6c525</t>
+          <t>d15393a8-4e0a-4b7e-b5f6-14bd2e41da30</t>
         </is>
       </c>
       <c r="B474" t="n">
@@ -16565,7 +16565,7 @@
     <row r="475">
       <c r="A475" s="1" t="inlineStr">
         <is>
-          <t>fe301c09-f0d2-4902-b24d-deb59793b5a0</t>
+          <t>4a82c4a7-ea73-4a8f-8cc4-e0d40f2fa33f</t>
         </is>
       </c>
       <c r="B475" t="n">
@@ -16599,7 +16599,7 @@
     <row r="476">
       <c r="A476" s="1" t="inlineStr">
         <is>
-          <t>74a7abc7-03f0-4213-97e0-3459523a569f</t>
+          <t>2ecf76d1-3937-4be2-9dd6-4f5124b965cb</t>
         </is>
       </c>
       <c r="B476" t="n">
@@ -16633,7 +16633,7 @@
     <row r="477">
       <c r="A477" s="1" t="inlineStr">
         <is>
-          <t>c277b978-7b89-490d-b8db-2e3ce8fd188d</t>
+          <t>c845b4ad-3105-4e09-b3ff-ef75b274670c</t>
         </is>
       </c>
       <c r="B477" t="n">
@@ -16667,7 +16667,7 @@
     <row r="478">
       <c r="A478" s="1" t="inlineStr">
         <is>
-          <t>ff183028-25bb-4ab0-a64d-95ede640981a</t>
+          <t>604334cc-76b0-4f01-815b-a2c51a6f262d</t>
         </is>
       </c>
       <c r="B478" t="n">
@@ -16701,7 +16701,7 @@
     <row r="479">
       <c r="A479" s="1" t="inlineStr">
         <is>
-          <t>a69c70cc-5460-4673-b88b-be6f2143df47</t>
+          <t>002b4c36-1bc3-4ed0-a657-8b9db9864151</t>
         </is>
       </c>
       <c r="B479" t="n">
@@ -16735,7 +16735,7 @@
     <row r="480">
       <c r="A480" s="1" t="inlineStr">
         <is>
-          <t>9b444765-d923-4832-b8ab-62a397f6cb64</t>
+          <t>2c2f7ef5-6f57-4b13-8d56-f7b49f8d9823</t>
         </is>
       </c>
       <c r="B480" t="n">
@@ -16769,7 +16769,7 @@
     <row r="481">
       <c r="A481" s="1" t="inlineStr">
         <is>
-          <t>46a83be3-9354-4cde-9ba0-a20ff30ad265</t>
+          <t>4c54168c-6c0e-4d3a-9971-87eb0196a740</t>
         </is>
       </c>
       <c r="B481" t="n">
@@ -16803,7 +16803,7 @@
     <row r="482">
       <c r="A482" s="1" t="inlineStr">
         <is>
-          <t>fc24e177-e533-466d-97bc-ab7035efcdd5</t>
+          <t>95ee8c60-3bfc-4a1b-8179-751f807600c9</t>
         </is>
       </c>
       <c r="B482" t="n">
@@ -16837,7 +16837,7 @@
     <row r="483">
       <c r="A483" s="1" t="inlineStr">
         <is>
-          <t>89b6b217-369f-4462-9c28-ae2a05fd78d7</t>
+          <t>83551d32-01f8-4bd5-86f0-6bc78704b64b</t>
         </is>
       </c>
       <c r="B483" t="n">
@@ -16871,7 +16871,7 @@
     <row r="484">
       <c r="A484" s="1" t="inlineStr">
         <is>
-          <t>082a80a2-a4bc-4d68-ab8e-19dfae181ae2</t>
+          <t>77e54425-2358-461b-bf71-7c13f24751c0</t>
         </is>
       </c>
       <c r="B484" t="n">
@@ -16905,7 +16905,7 @@
     <row r="485">
       <c r="A485" s="1" t="inlineStr">
         <is>
-          <t>f4f52c1e-58a6-4dd6-adad-82f37ad6f5ee</t>
+          <t>02e47103-59a6-4e5e-9eba-6b7939731771</t>
         </is>
       </c>
       <c r="B485" t="n">
@@ -16939,7 +16939,7 @@
     <row r="486">
       <c r="A486" s="1" t="inlineStr">
         <is>
-          <t>73693b4e-a227-4d12-a986-bbfcdbc8dc37</t>
+          <t>526875c9-4a63-44c4-8559-a18d9292f83f</t>
         </is>
       </c>
       <c r="B486" t="n">
@@ -16973,7 +16973,7 @@
     <row r="487">
       <c r="A487" s="1" t="inlineStr">
         <is>
-          <t>6d973339-4905-47f8-a66e-06142fba18d9</t>
+          <t>8ce4384b-f416-47b1-b2e7-3cffdc7a5524</t>
         </is>
       </c>
       <c r="B487" t="n">
@@ -17007,7 +17007,7 @@
     <row r="488">
       <c r="A488" s="1" t="inlineStr">
         <is>
-          <t>472a8d40-4514-4bf3-ac0f-c0e886cf39e4</t>
+          <t>3273b584-944d-4e93-b08a-c6188b567a3d</t>
         </is>
       </c>
       <c r="B488" t="n">
@@ -17041,7 +17041,7 @@
     <row r="489">
       <c r="A489" s="1" t="inlineStr">
         <is>
-          <t>38258c6c-4666-4ac1-a48e-42362f9536d5</t>
+          <t>02ae57a1-6b47-43c9-81f0-d7c67b170db1</t>
         </is>
       </c>
       <c r="B489" t="n">
@@ -17075,7 +17075,7 @@
     <row r="490">
       <c r="A490" s="1" t="inlineStr">
         <is>
-          <t>a01797fb-7b85-4fb3-b23c-9c2f564291f5</t>
+          <t>b186c83d-ccb8-4ed6-8f8c-edb7485a0af9</t>
         </is>
       </c>
       <c r="B490" t="n">
@@ -17109,7 +17109,7 @@
     <row r="491">
       <c r="A491" s="1" t="inlineStr">
         <is>
-          <t>905da2e8-785a-4b20-ab04-0ab634c62d4a</t>
+          <t>d815717d-4220-4455-ac86-0d525cb699f2</t>
         </is>
       </c>
       <c r="B491" t="n">
@@ -17143,7 +17143,7 @@
     <row r="492">
       <c r="A492" s="1" t="inlineStr">
         <is>
-          <t>d86a1b33-bdf6-4158-b5d7-8980efc5e4d7</t>
+          <t>46cf2f03-54e2-491c-bed5-f5a71a608bce</t>
         </is>
       </c>
       <c r="B492" t="n">
@@ -17177,7 +17177,7 @@
     <row r="493">
       <c r="A493" s="1" t="inlineStr">
         <is>
-          <t>2d28e2b9-eae1-42cd-8be9-2797e43e0822</t>
+          <t>6607bc03-b2e8-44e3-a6cb-880a2a5f05f6</t>
         </is>
       </c>
       <c r="B493" t="n">
@@ -17211,7 +17211,7 @@
     <row r="494">
       <c r="A494" s="1" t="inlineStr">
         <is>
-          <t>64d2e6c0-2865-4b7e-a87d-d16d631975e1</t>
+          <t>8eb567d1-99c8-4e95-824a-ea7f53ff40a3</t>
         </is>
       </c>
       <c r="B494" t="n">
@@ -17245,7 +17245,7 @@
     <row r="495">
       <c r="A495" s="1" t="inlineStr">
         <is>
-          <t>4176e34f-8217-4c84-aaea-1ff748fc8734</t>
+          <t>4592fca0-06f0-4140-a01e-c2902eb06728</t>
         </is>
       </c>
       <c r="B495" t="n">
@@ -17279,7 +17279,7 @@
     <row r="496">
       <c r="A496" s="1" t="inlineStr">
         <is>
-          <t>1e51ba33-311d-4b5b-87b2-b8478f2e48d2</t>
+          <t>32e5deb1-aeb9-4c17-92b7-3737b77c48f8</t>
         </is>
       </c>
       <c r="B496" t="n">
@@ -17313,7 +17313,7 @@
     <row r="497">
       <c r="A497" s="1" t="inlineStr">
         <is>
-          <t>9f0fa896-c926-4e81-a693-f2b80e7dbe6f</t>
+          <t>1ce70443-379f-4c3e-bec3-60cef0270c4e</t>
         </is>
       </c>
       <c r="B497" t="n">
@@ -17347,7 +17347,7 @@
     <row r="498">
       <c r="A498" s="1" t="inlineStr">
         <is>
-          <t>0e6f6ef9-49eb-4bdf-9cc2-51a71c932506</t>
+          <t>b673a5a9-0d1c-4c50-9cce-b5a21456816b</t>
         </is>
       </c>
       <c r="B498" t="n">
@@ -17381,7 +17381,7 @@
     <row r="499">
       <c r="A499" s="1" t="inlineStr">
         <is>
-          <t>7e5e4931-deac-4427-942b-97ebaf065291</t>
+          <t>04beefe2-8c0e-4cf0-9673-46ffebb15cc7</t>
         </is>
       </c>
       <c r="B499" t="n">
@@ -17415,7 +17415,7 @@
     <row r="500">
       <c r="A500" s="1" t="inlineStr">
         <is>
-          <t>9cf9e906-15e2-41a9-8531-8e07f235c750</t>
+          <t>056292dc-6dfd-45fd-852b-f5a85fa9ba24</t>
         </is>
       </c>
       <c r="B500" t="n">
@@ -17449,7 +17449,7 @@
     <row r="501">
       <c r="A501" s="1" t="inlineStr">
         <is>
-          <t>db8a6134-d6ca-4864-9ff2-65c555985561</t>
+          <t>3da66efd-a1f1-4f93-ba06-cfb85ca9b5f7</t>
         </is>
       </c>
       <c r="B501" t="n">
@@ -17483,7 +17483,7 @@
     <row r="502">
       <c r="A502" s="1" t="inlineStr">
         <is>
-          <t>c381413c-0271-454a-b8b3-d45f31687f58</t>
+          <t>920832a3-1bf5-4462-8b85-afcd9db0f3f8</t>
         </is>
       </c>
       <c r="B502" t="n">
@@ -17517,7 +17517,7 @@
     <row r="503">
       <c r="A503" s="1" t="inlineStr">
         <is>
-          <t>30b991f5-c0c9-4893-beb6-54f08437aa5a</t>
+          <t>f380d71e-0b05-41fe-82aa-4f0312695aa3</t>
         </is>
       </c>
       <c r="B503" t="n">
@@ -17551,7 +17551,7 @@
     <row r="504">
       <c r="A504" s="1" t="inlineStr">
         <is>
-          <t>3f145310-8c3f-4acf-8952-73667010d818</t>
+          <t>1736f6e3-288d-41b5-a125-bb9b988dec89</t>
         </is>
       </c>
       <c r="B504" t="n">
@@ -17585,7 +17585,7 @@
     <row r="505">
       <c r="A505" s="1" t="inlineStr">
         <is>
-          <t>890c4cad-daa7-48b5-b4da-28964ecaeade</t>
+          <t>71fc8696-dbdf-4dbd-b564-ce5cf01e7319</t>
         </is>
       </c>
       <c r="B505" t="n">
@@ -17619,7 +17619,7 @@
     <row r="506">
       <c r="A506" s="1" t="inlineStr">
         <is>
-          <t>5d874601-abd8-47e1-9b81-9f2445f70268</t>
+          <t>65d4e4a4-1708-4c07-8fa5-d625b1fed857</t>
         </is>
       </c>
       <c r="B506" t="n">
@@ -17653,7 +17653,7 @@
     <row r="507">
       <c r="A507" s="1" t="inlineStr">
         <is>
-          <t>4a0f2f81-84e9-46aa-bfc0-fbaff9ed1163</t>
+          <t>7d5f2b6f-16a2-4f29-886e-78328c291ceb</t>
         </is>
       </c>
       <c r="B507" t="n">
@@ -17687,7 +17687,7 @@
     <row r="508">
       <c r="A508" s="1" t="inlineStr">
         <is>
-          <t>1b5fd83b-838f-43f4-a39b-6af27eaa181c</t>
+          <t>0ce43f17-25dc-4028-8d79-7f8545bcc084</t>
         </is>
       </c>
       <c r="B508" t="n">
@@ -17721,7 +17721,7 @@
     <row r="509">
       <c r="A509" s="1" t="inlineStr">
         <is>
-          <t>3295b093-10e6-468c-b539-412b9b619c2e</t>
+          <t>f0f97fd2-9339-4922-be0c-43305fc8d43a</t>
         </is>
       </c>
       <c r="B509" t="n">
@@ -17755,7 +17755,7 @@
     <row r="510">
       <c r="A510" s="1" t="inlineStr">
         <is>
-          <t>3d3160f2-a730-4f84-a812-3ba1281dbbc0</t>
+          <t>efeef223-7dad-44cf-9d9a-4a89c7f5aedf</t>
         </is>
       </c>
       <c r="B510" t="n">
@@ -17789,7 +17789,7 @@
     <row r="511">
       <c r="A511" s="1" t="inlineStr">
         <is>
-          <t>f7d5db69-63f4-4a1d-924e-efb69a0235e2</t>
+          <t>ae3c2315-6559-4995-b404-1a963a4ba3f7</t>
         </is>
       </c>
       <c r="B511" t="n">
@@ -17823,7 +17823,7 @@
     <row r="512">
       <c r="A512" s="1" t="inlineStr">
         <is>
-          <t>8371a0c9-4898-4d78-9d53-0a72201a8c99</t>
+          <t>048294d6-993f-4f3f-b086-9673a0a71cc7</t>
         </is>
       </c>
       <c r="B512" t="n">
@@ -17857,7 +17857,7 @@
     <row r="513">
       <c r="A513" s="1" t="inlineStr">
         <is>
-          <t>1d52327d-19ca-42c3-b5e4-fc6e1cb65328</t>
+          <t>71ef6e38-8d88-4d19-9e56-c502ff3919fb</t>
         </is>
       </c>
       <c r="B513" t="n">
@@ -17891,7 +17891,7 @@
     <row r="514">
       <c r="A514" s="1" t="inlineStr">
         <is>
-          <t>4c564018-e47d-4aff-b1e4-90625f3bfa7a</t>
+          <t>e9556d50-7f11-481d-ab70-4ff845c70382</t>
         </is>
       </c>
       <c r="B514" t="n">
@@ -17925,7 +17925,7 @@
     <row r="515">
       <c r="A515" s="1" t="inlineStr">
         <is>
-          <t>f7573bb0-3565-40bc-a1b1-92e5bb607d64</t>
+          <t>d4702733-bd07-4e2f-ab6e-213526d83837</t>
         </is>
       </c>
       <c r="B515" t="n">
@@ -17959,7 +17959,7 @@
     <row r="516">
       <c r="A516" s="1" t="inlineStr">
         <is>
-          <t>e6960726-fd60-441a-868d-cd4644ce1230</t>
+          <t>cef295fa-aaf5-42c3-9be0-cc32393b890e</t>
         </is>
       </c>
       <c r="B516" t="n">
@@ -17993,7 +17993,7 @@
     <row r="517">
       <c r="A517" s="1" t="inlineStr">
         <is>
-          <t>ab03aea6-e6c7-40e2-8a04-cb4c46c0ad20</t>
+          <t>1978b57e-f57d-455a-99fa-b303737675e0</t>
         </is>
       </c>
       <c r="B517" t="n">
@@ -18027,7 +18027,7 @@
     <row r="518">
       <c r="A518" s="1" t="inlineStr">
         <is>
-          <t>d0a455d3-b524-4c63-aeb2-e86028b9410a</t>
+          <t>e29dad0e-9d69-4c9e-949e-63313c5c6090</t>
         </is>
       </c>
       <c r="B518" t="n">
@@ -18061,7 +18061,7 @@
     <row r="519">
       <c r="A519" s="1" t="inlineStr">
         <is>
-          <t>4b0a420b-112d-4977-9ff2-a2d15a22c734</t>
+          <t>be865b18-9ee6-46cc-ac46-b95a3dbacd48</t>
         </is>
       </c>
       <c r="B519" t="n">
@@ -18095,7 +18095,7 @@
     <row r="520">
       <c r="A520" s="1" t="inlineStr">
         <is>
-          <t>8ee9b73f-b5dc-47b1-beb9-16fe366f5da3</t>
+          <t>bd19cfe8-27e4-4779-855c-09da87e2f7b4</t>
         </is>
       </c>
       <c r="B520" t="n">
@@ -18129,7 +18129,7 @@
     <row r="521">
       <c r="A521" s="1" t="inlineStr">
         <is>
-          <t>7fd74b7e-7172-4b7e-a2f2-f003301a39d3</t>
+          <t>1b35db3a-b45c-4132-97bf-d4fb9ec75afc</t>
         </is>
       </c>
       <c r="B521" t="n">
@@ -18163,7 +18163,7 @@
     <row r="522">
       <c r="A522" s="1" t="inlineStr">
         <is>
-          <t>f563109f-1fb4-4484-97ac-9c79996f228b</t>
+          <t>9b5565de-cc13-4626-abbf-3679e73173ac</t>
         </is>
       </c>
       <c r="B522" t="n">
@@ -18197,7 +18197,7 @@
     <row r="523">
       <c r="A523" s="1" t="inlineStr">
         <is>
-          <t>25b6adb8-0cff-404b-8290-c1c07369cb33</t>
+          <t>d7792c29-13fa-46aa-9803-bb920101da0a</t>
         </is>
       </c>
       <c r="B523" t="n">
@@ -18231,7 +18231,7 @@
     <row r="524">
       <c r="A524" s="1" t="inlineStr">
         <is>
-          <t>8de347b6-870c-4cfd-812f-d4598d9d0e4e</t>
+          <t>eb862691-a476-495e-ba2e-74e522490165</t>
         </is>
       </c>
       <c r="B524" t="n">
@@ -18265,7 +18265,7 @@
     <row r="525">
       <c r="A525" s="1" t="inlineStr">
         <is>
-          <t>5e04b870-b7b5-4eff-bf88-47680a506ec1</t>
+          <t>227d4305-208d-4411-a5e9-cc33fcf07b59</t>
         </is>
       </c>
       <c r="B525" t="n">
@@ -18299,7 +18299,7 @@
     <row r="526">
       <c r="A526" s="1" t="inlineStr">
         <is>
-          <t>41f0f229-e578-4fe8-b266-3cca534b1f94</t>
+          <t>d6ddb6e7-18b1-47a1-9c44-c5b640c6f5b2</t>
         </is>
       </c>
       <c r="B526" t="n">
@@ -18333,7 +18333,7 @@
     <row r="527">
       <c r="A527" s="1" t="inlineStr">
         <is>
-          <t>e8d4d414-a8a7-42eb-a7bd-111f87bc02fd</t>
+          <t>b781922d-f261-45da-8ca6-c5ef75290d8a</t>
         </is>
       </c>
       <c r="B527" t="n">
@@ -18367,7 +18367,7 @@
     <row r="528">
       <c r="A528" s="1" t="inlineStr">
         <is>
-          <t>fcebd451-9b5f-478a-bf87-6cafb366ace9</t>
+          <t>3a7e736c-ff5a-45d3-be0e-987b9ef6960a</t>
         </is>
       </c>
       <c r="B528" t="n">
@@ -18401,7 +18401,7 @@
     <row r="529">
       <c r="A529" s="1" t="inlineStr">
         <is>
-          <t>a9eb82e1-cfc5-4716-878a-ba87a209d34d</t>
+          <t>89246b4b-2724-4d94-bf85-a8008458970b</t>
         </is>
       </c>
       <c r="B529" t="n">
@@ -18435,7 +18435,7 @@
     <row r="530">
       <c r="A530" s="1" t="inlineStr">
         <is>
-          <t>f69278a6-8ec5-44d2-a040-1a5cc4267cdf</t>
+          <t>293b2694-5f0e-44b3-a595-72f88418d485</t>
         </is>
       </c>
       <c r="B530" t="n">
@@ -18469,7 +18469,7 @@
     <row r="531">
       <c r="A531" s="1" t="inlineStr">
         <is>
-          <t>2b9227c6-337b-4e88-bc99-eae710c64276</t>
+          <t>5d30ba05-ce67-4bb1-b13f-ea9f0fb062d5</t>
         </is>
       </c>
       <c r="B531" t="n">
@@ -18503,7 +18503,7 @@
     <row r="532">
       <c r="A532" s="1" t="inlineStr">
         <is>
-          <t>e31d96cf-b110-4c54-b6ae-8de6a39d3f26</t>
+          <t>633391e0-ecd3-4d3b-a344-a07868690067</t>
         </is>
       </c>
       <c r="B532" t="n">
@@ -18537,7 +18537,7 @@
     <row r="533">
       <c r="A533" s="1" t="inlineStr">
         <is>
-          <t>263659d6-05e1-4d71-84a7-7aa33bd905a7</t>
+          <t>82c63d5b-4deb-4a8f-a29b-6b8d9f730214</t>
         </is>
       </c>
       <c r="B533" t="n">
@@ -18571,7 +18571,7 @@
     <row r="534">
       <c r="A534" s="1" t="inlineStr">
         <is>
-          <t>3b74dfa4-cdd6-4723-a5f4-6256023e7570</t>
+          <t>f25fdc4b-0a3b-4130-81f5-2c8ddcf33250</t>
         </is>
       </c>
       <c r="B534" t="n">

</xml_diff>